<commit_message>
code refactor for Array
</commit_message>
<xml_diff>
--- a/Stock/US_Stock.xlsx
+++ b/Stock/US_Stock.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA84AD7-5C84-4774-AAD1-3F4AEFE91DE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8544F9-ACF5-4EAD-AE83-E3BCDCE24169}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technology" sheetId="14" r:id="rId1"/>
@@ -43,14 +43,14 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -2227,7 +2227,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2382,6 +2382,12 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2700,33 +2706,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3B4BCA-42DA-4C85-9005-E70B6BE65D74}">
   <dimension ref="A1:V71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="12" width="23.53515625" customWidth="1"/>
-    <col min="13" max="13" width="22.3046875" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="12" width="23.52734375" customWidth="1"/>
+    <col min="13" max="13" width="22.29296875" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -2798,117 +2804,117 @@
       <c r="A2" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="54" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="55">
+      <c r="H2" s="111">
         <v>1360</v>
       </c>
-      <c r="I2" s="55">
+      <c r="I2" s="111">
         <v>40.58</v>
       </c>
-      <c r="J2" s="56">
+      <c r="J2" s="109">
         <v>31.11</v>
       </c>
-      <c r="K2" s="56">
+      <c r="K2" s="109">
         <v>14.47</v>
       </c>
-      <c r="L2" s="56">
+      <c r="L2" s="109">
         <v>24.21</v>
       </c>
-      <c r="M2" s="56">
+      <c r="M2" s="109">
         <v>21.96</v>
       </c>
-      <c r="N2" s="56">
+      <c r="N2" s="109">
         <v>10.16</v>
       </c>
-      <c r="O2" s="57">
+      <c r="O2" s="112">
         <v>7.8E-2</v>
       </c>
-      <c r="P2" s="57">
+      <c r="P2" s="112">
         <v>0.14069999999999999</v>
       </c>
-      <c r="Q2" s="57">
+      <c r="Q2" s="112">
         <v>0.45700000000000002</v>
       </c>
-      <c r="R2" s="57">
+      <c r="R2" s="112">
         <v>0.4289</v>
       </c>
-      <c r="S2" s="57">
+      <c r="S2" s="112">
         <v>0.79149999999999998</v>
       </c>
-      <c r="T2" s="56">
+      <c r="T2" s="109">
         <v>2.77</v>
       </c>
-      <c r="U2" s="55">
+      <c r="U2" s="111">
         <v>963190</v>
       </c>
-      <c r="V2" s="68" t="s">
+      <c r="V2" s="113" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="18"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="54" t="s">
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="55">
+      <c r="H3" s="111">
         <v>1180</v>
       </c>
-      <c r="I3" s="55">
+      <c r="I3" s="111">
         <v>21.65</v>
       </c>
-      <c r="J3" s="56">
+      <c r="J3" s="109">
         <v>103.22</v>
       </c>
-      <c r="K3" s="56">
+      <c r="K3" s="109">
         <v>21.36</v>
       </c>
-      <c r="L3" s="56">
+      <c r="L3" s="109">
         <v>35.200000000000003</v>
       </c>
-      <c r="M3" s="56">
+      <c r="M3" s="109">
         <v>31.65</v>
       </c>
-      <c r="N3" s="56">
+      <c r="N3" s="109">
         <v>4.1900000000000004</v>
       </c>
-      <c r="O3" s="57">
+      <c r="O3" s="112">
         <v>0.2581</v>
       </c>
-      <c r="P3" s="57">
+      <c r="P3" s="112">
         <v>0.50409999999999999</v>
       </c>
-      <c r="Q3" s="57">
+      <c r="Q3" s="112">
         <v>0.13020000000000001</v>
       </c>
-      <c r="R3" s="57">
+      <c r="R3" s="112">
         <v>0.2107</v>
       </c>
-      <c r="S3" s="57">
+      <c r="S3" s="112">
         <v>1.2494000000000001</v>
       </c>
-      <c r="T3" s="56">
+      <c r="T3" s="109">
         <v>2.12</v>
       </c>
-      <c r="U3" s="55">
+      <c r="U3" s="111">
         <v>371270</v>
       </c>
-      <c r="V3" s="68" t="s">
+      <c r="V3" s="113" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3048,10 +3054,10 @@
       <c r="G6" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="88">
+      <c r="H6" s="103">
         <v>511.19</v>
       </c>
-      <c r="I6" s="88">
+      <c r="I6" s="103">
         <v>21.21</v>
       </c>
       <c r="J6" s="88">
@@ -3069,25 +3075,25 @@
       <c r="N6" s="88">
         <v>7.24</v>
       </c>
-      <c r="O6" s="88">
+      <c r="O6" s="101">
         <v>0.41489999999999999</v>
       </c>
-      <c r="P6" s="88">
+      <c r="P6" s="101">
         <v>0.42099999999999999</v>
       </c>
-      <c r="Q6" s="88">
+      <c r="Q6" s="101">
         <v>0.49120000000000003</v>
       </c>
-      <c r="R6" s="88">
+      <c r="R6" s="101">
         <v>0.19969999999999999</v>
       </c>
-      <c r="S6" s="88">
+      <c r="S6" s="101">
         <v>0.10489999999999999</v>
       </c>
       <c r="T6" s="88">
         <v>4.67</v>
       </c>
-      <c r="U6" s="88">
+      <c r="U6" s="108">
         <v>1632260</v>
       </c>
       <c r="V6" s="84" t="s">
@@ -3244,7 +3250,7 @@
       <c r="G10" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="H10" s="93">
+      <c r="H10" s="97">
         <v>68.739999999999995</v>
       </c>
       <c r="I10" s="93"/>
@@ -3259,25 +3265,25 @@
       <c r="N10" s="93">
         <v>42.63</v>
       </c>
-      <c r="O10" s="93">
+      <c r="O10" s="96">
         <v>0.71940000000000004</v>
       </c>
-      <c r="P10" s="93">
+      <c r="P10" s="96">
         <v>0.38279999999999997</v>
       </c>
-      <c r="Q10" s="93">
+      <c r="Q10" s="96">
         <v>-6.6799999999999998E-2</v>
       </c>
-      <c r="R10" s="93">
+      <c r="R10" s="96">
         <v>-4.9299999999999997E-2</v>
       </c>
-      <c r="S10" s="93">
+      <c r="S10" s="96">
         <v>5.0299999999999997E-2</v>
       </c>
       <c r="T10" s="93">
         <v>10.65</v>
       </c>
-      <c r="U10" s="93">
+      <c r="U10" s="95">
         <v>315630</v>
       </c>
       <c r="V10" s="89" t="s">
@@ -3296,10 +3302,10 @@
       <c r="G11" s="82" t="s">
         <v>174</v>
       </c>
-      <c r="H11" s="82">
+      <c r="H11" s="91">
         <v>11.1</v>
       </c>
-      <c r="I11" s="82">
+      <c r="I11" s="81">
         <v>2.4E-2</v>
       </c>
       <c r="J11" s="82">
@@ -3317,25 +3323,25 @@
       <c r="N11" s="82">
         <v>16.62</v>
       </c>
-      <c r="O11" s="82">
+      <c r="O11" s="83">
         <v>0.71509999999999996</v>
       </c>
-      <c r="P11" s="82">
+      <c r="P11" s="83">
         <v>1.8495999999999999</v>
       </c>
-      <c r="Q11" s="82">
+      <c r="Q11" s="83">
         <v>0.20250000000000001</v>
       </c>
-      <c r="R11" s="82">
+      <c r="R11" s="83">
         <v>0.2094</v>
       </c>
-      <c r="S11" s="82">
+      <c r="S11" s="83">
         <v>0.30930000000000002</v>
       </c>
       <c r="T11" s="82">
         <v>1.61</v>
       </c>
-      <c r="U11" s="82">
+      <c r="U11" s="81">
         <v>504620</v>
       </c>
       <c r="V11" s="84" t="s">
@@ -3387,7 +3393,7 @@
       <c r="T12" s="45">
         <v>2.62</v>
       </c>
-      <c r="U12" s="74">
+      <c r="U12" s="98">
         <v>684190</v>
       </c>
       <c r="V12" s="13" t="s">
@@ -3402,10 +3408,10 @@
       <c r="G13" t="s">
         <v>71</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="69">
         <v>7.92</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="69">
         <v>2.274E-2</v>
       </c>
       <c r="J13">
@@ -3423,25 +3429,25 @@
       <c r="N13">
         <v>18.55</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="46">
         <v>0.50670000000000004</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="46">
         <v>0.11360000000000001</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="46">
         <v>0.111</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="46">
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="46">
         <v>1.7283999999999999</v>
       </c>
       <c r="T13">
         <v>2.8</v>
       </c>
-      <c r="U13" s="76">
+      <c r="U13" s="69">
         <v>348260</v>
       </c>
       <c r="V13" s="13" t="s">
@@ -3493,7 +3499,7 @@
       <c r="T14" s="45">
         <v>1.1200000000000001</v>
       </c>
-      <c r="U14" s="74">
+      <c r="U14" s="98">
         <v>419880</v>
       </c>
       <c r="V14" s="13" t="s">
@@ -3545,7 +3551,7 @@
       <c r="T15" s="45">
         <v>8.56</v>
       </c>
-      <c r="U15" s="74">
+      <c r="U15" s="98">
         <v>390520</v>
       </c>
       <c r="V15" s="13" t="s">
@@ -3601,7 +3607,7 @@
       <c r="T16" s="12">
         <v>3.63</v>
       </c>
-      <c r="U16" s="44">
+      <c r="U16" s="24">
         <v>245920</v>
       </c>
       <c r="V16" s="13" t="s">
@@ -6214,13 +6220,13 @@
       <selection activeCell="U191" sqref="U191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.234375" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="4" width="9.23046875" style="62"/>
-    <col min="5" max="5" width="12.61328125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="9.23046875" style="62"/>
-    <col min="7" max="7" width="14.765625" style="62" customWidth="1"/>
-    <col min="8" max="16384" width="9.23046875" style="62"/>
+    <col min="1" max="4" width="9.234375" style="62"/>
+    <col min="5" max="5" width="12.5859375" style="62" customWidth="1"/>
+    <col min="6" max="6" width="9.234375" style="62"/>
+    <col min="7" max="7" width="14.76171875" style="62" customWidth="1"/>
+    <col min="8" max="16384" width="9.234375" style="62"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -30448,7 +30454,7 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
@@ -34138,28 +34144,28 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -35171,28 +35177,28 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="21.15234375" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="21.17578125" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -38653,29 +38659,29 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.765625" customWidth="1"/>
+    <col min="1" max="1" width="20.76171875" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="20" width="23.765625" customWidth="1"/>
-    <col min="21" max="21" width="23.765625" style="76" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="20" width="23.76171875" customWidth="1"/>
+    <col min="21" max="21" width="23.76171875" style="76" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -39605,28 +39611,28 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -40366,28 +40372,28 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -41608,32 +41614,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7612E97-4D94-4070-BE89-A5C4CC24AB2D}">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -42817,28 +42823,28 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -43882,28 +43888,28 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.23046875" customWidth="1"/>
+    <col min="1" max="1" width="15.234375" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="12.84375" hidden="1" customWidth="1"/>
-    <col min="4" max="6" width="20.765625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.765625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.3046875" customWidth="1"/>
-    <col min="11" max="11" width="13.765625" customWidth="1"/>
-    <col min="12" max="13" width="23.53515625" customWidth="1"/>
-    <col min="14" max="14" width="20.23046875" customWidth="1"/>
-    <col min="15" max="15" width="30.07421875" customWidth="1"/>
-    <col min="16" max="16" width="39.23046875" customWidth="1"/>
-    <col min="17" max="18" width="23.765625" customWidth="1"/>
-    <col min="19" max="19" width="27.765625" customWidth="1"/>
-    <col min="20" max="21" width="23.765625" customWidth="1"/>
-    <col min="22" max="22" width="76.07421875" customWidth="1"/>
+    <col min="3" max="3" width="12.8203125" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="20.76171875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.52734375" customWidth="1"/>
+    <col min="8" max="8" width="16.234375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.76171875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="13.76171875" customWidth="1"/>
+    <col min="12" max="13" width="23.52734375" customWidth="1"/>
+    <col min="14" max="14" width="20.234375" customWidth="1"/>
+    <col min="15" max="15" width="30.05859375" customWidth="1"/>
+    <col min="16" max="16" width="39.234375" customWidth="1"/>
+    <col min="17" max="18" width="23.76171875" customWidth="1"/>
+    <col min="19" max="19" width="27.76171875" customWidth="1"/>
+    <col min="20" max="21" width="23.76171875" customWidth="1"/>
+    <col min="22" max="22" width="76.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" ht="15.75">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Code refactor for Binary Tree
</commit_message>
<xml_diff>
--- a/Stock/US_Stock.xlsx
+++ b/Stock/US_Stock.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3C2FC6-9D6E-4666-ABE6-D5595D0DC86D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF74D9F7-F7B5-44D7-AD47-184274BE309F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="649">
   <si>
     <t>代码</t>
   </si>
@@ -1971,6 +1971,48 @@
   </si>
   <si>
     <t>LRCX</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>IQIYI INC</t>
+  </si>
+  <si>
+    <t>IQ</t>
+  </si>
+  <si>
+    <t>58.COM INC</t>
+  </si>
+  <si>
+    <t>WUBA</t>
+  </si>
+  <si>
+    <t>Commnunity</t>
+  </si>
+  <si>
+    <t>HUYA INC</t>
+  </si>
+  <si>
+    <t>HUYA</t>
+  </si>
+  <si>
+    <t>Live Show</t>
+  </si>
+  <si>
+    <t>DOUYU INTERNATIONAL</t>
+  </si>
+  <si>
+    <t>DOYU</t>
+  </si>
+  <si>
+    <t>BILIBILI INC</t>
+  </si>
+  <si>
+    <t>BILI</t>
+  </si>
+  <si>
+    <t>Streaming Video</t>
   </si>
 </sst>
 </file>
@@ -2710,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3B4BCA-42DA-4C85-9005-E70B6BE65D74}">
-  <dimension ref="A1:V71"/>
+  <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q41" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="W67" sqref="W67"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection sqref="A1:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3246,7 +3288,7 @@
       <c r="A10" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="93" t="s">
+      <c r="B10" s="92" t="s">
         <v>67</v>
       </c>
       <c r="C10" s="93"/>
@@ -3298,7 +3340,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="31"/>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="86" t="s">
         <v>173</v>
       </c>
       <c r="C11" s="82"/>
@@ -6211,6 +6253,400 @@
       <c r="T71" s="15"/>
       <c r="U71" s="53"/>
       <c r="V71" s="16"/>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="A72" s="31" t="s">
+        <v>635</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>636</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="28" t="s">
+        <v>637</v>
+      </c>
+      <c r="H72" s="38">
+        <v>13.17</v>
+      </c>
+      <c r="I72" s="38">
+        <v>0.45469999999999999</v>
+      </c>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9">
+        <v>6.79</v>
+      </c>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9">
+        <v>-8.5</v>
+      </c>
+      <c r="N72" s="9">
+        <v>3.14</v>
+      </c>
+      <c r="O72" s="20">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="P72" s="20">
+        <v>0.1802</v>
+      </c>
+      <c r="Q72" s="20"/>
+      <c r="R72" s="20">
+        <v>-0.77149999999999996</v>
+      </c>
+      <c r="S72" s="20">
+        <v>1.7843</v>
+      </c>
+      <c r="T72" s="9">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="U72" s="43">
+        <v>468440</v>
+      </c>
+      <c r="V72" s="10" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22">
+      <c r="A73" s="31"/>
+      <c r="B73" s="11" t="s">
+        <v>638</v>
+      </c>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="34" t="s">
+        <v>639</v>
+      </c>
+      <c r="H73" s="24">
+        <v>7.76</v>
+      </c>
+      <c r="I73" s="24">
+        <v>0.60858999999999996</v>
+      </c>
+      <c r="J73" s="42">
+        <v>6.58</v>
+      </c>
+      <c r="K73" s="42">
+        <v>1.97</v>
+      </c>
+      <c r="L73" s="42">
+        <v>6.51</v>
+      </c>
+      <c r="M73" s="42">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N73" s="42">
+        <v>3.46</v>
+      </c>
+      <c r="O73" s="21">
+        <v>0.53210000000000002</v>
+      </c>
+      <c r="P73" s="21">
+        <v>1.1326000000000001</v>
+      </c>
+      <c r="Q73" s="21"/>
+      <c r="R73" s="21">
+        <v>0.30220000000000002</v>
+      </c>
+      <c r="S73" s="21">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="T73" s="45">
+        <v>1.65</v>
+      </c>
+      <c r="U73" s="74">
+        <v>102890</v>
+      </c>
+      <c r="V73" s="13" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22">
+      <c r="A74" s="31"/>
+      <c r="B74" s="11" t="s">
+        <v>641</v>
+      </c>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="34" t="s">
+        <v>642</v>
+      </c>
+      <c r="H74" s="24">
+        <v>3.76</v>
+      </c>
+      <c r="I74" s="24">
+        <v>0.27065</v>
+      </c>
+      <c r="J74" s="42">
+        <v>57.1</v>
+      </c>
+      <c r="K74" s="42">
+        <v>3.3</v>
+      </c>
+      <c r="L74" s="42">
+        <v>54.83</v>
+      </c>
+      <c r="M74" s="42">
+        <v>39.01</v>
+      </c>
+      <c r="N74" s="42">
+        <v>3.07</v>
+      </c>
+      <c r="O74" s="21">
+        <v>0.5998</v>
+      </c>
+      <c r="P74" s="21">
+        <v>-3.15E-2</v>
+      </c>
+      <c r="Q74" s="21"/>
+      <c r="R74" s="21">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="S74" s="21">
+        <v>1.17E-2</v>
+      </c>
+      <c r="T74" s="45">
+        <v>4.51</v>
+      </c>
+      <c r="U74" s="74">
+        <v>645340</v>
+      </c>
+      <c r="V74" s="13" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22">
+      <c r="A75" s="31"/>
+      <c r="B75" s="11" t="s">
+        <v>644</v>
+      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="34" t="s">
+        <v>645</v>
+      </c>
+      <c r="H75" s="24">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I75" s="24">
+        <v>0.11448</v>
+      </c>
+      <c r="J75" s="42">
+        <v>380</v>
+      </c>
+      <c r="K75" s="42">
+        <v>6.75</v>
+      </c>
+      <c r="L75" s="42">
+        <v>351.92</v>
+      </c>
+      <c r="M75" s="42">
+        <v>27.35</v>
+      </c>
+      <c r="N75" s="42">
+        <v>1.92</v>
+      </c>
+      <c r="O75" s="21">
+        <v>0.29260000000000003</v>
+      </c>
+      <c r="P75" s="21">
+        <v>-0.27039999999999997</v>
+      </c>
+      <c r="Q75" s="21"/>
+      <c r="R75" s="21">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="S75" s="21">
+        <v>0</v>
+      </c>
+      <c r="T75" s="45">
+        <v>3.77</v>
+      </c>
+      <c r="U75" s="74">
+        <v>536960</v>
+      </c>
+      <c r="V75" s="13" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22">
+      <c r="A76" s="31"/>
+      <c r="B76" s="11" t="s">
+        <v>646</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="34" t="s">
+        <v>647</v>
+      </c>
+      <c r="H76" s="24">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="I76" s="24">
+        <v>-1.4579999999999999E-2</v>
+      </c>
+      <c r="J76" s="42"/>
+      <c r="K76" s="42">
+        <v>9.15</v>
+      </c>
+      <c r="L76" s="42"/>
+      <c r="M76" s="42">
+        <v>-43.42</v>
+      </c>
+      <c r="N76" s="42">
+        <v>10.02</v>
+      </c>
+      <c r="O76" s="21">
+        <v>0.66810000000000003</v>
+      </c>
+      <c r="P76" s="21">
+        <v>-0.23899999999999999</v>
+      </c>
+      <c r="Q76" s="21"/>
+      <c r="R76" s="21">
+        <v>-0.1736</v>
+      </c>
+      <c r="S76" s="21">
+        <v>0.52510000000000001</v>
+      </c>
+      <c r="T76" s="45">
+        <v>2.42</v>
+      </c>
+      <c r="U76" s="74">
+        <v>203180</v>
+      </c>
+      <c r="V76" s="13" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22">
+      <c r="A77" s="31"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="34"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="42"/>
+      <c r="K77" s="42"/>
+      <c r="L77" s="42"/>
+      <c r="M77" s="42"/>
+      <c r="N77" s="42"/>
+      <c r="O77" s="21"/>
+      <c r="P77" s="21"/>
+      <c r="Q77" s="21"/>
+      <c r="R77" s="21"/>
+      <c r="S77" s="21"/>
+      <c r="T77" s="45"/>
+      <c r="U77" s="74"/>
+      <c r="V77" s="13"/>
+    </row>
+    <row r="78" spans="1:22">
+      <c r="A78" s="31"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="34"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="42"/>
+      <c r="K78" s="42"/>
+      <c r="L78" s="42"/>
+      <c r="M78" s="42"/>
+      <c r="N78" s="42"/>
+      <c r="O78" s="21"/>
+      <c r="P78" s="21"/>
+      <c r="Q78" s="21"/>
+      <c r="R78" s="21"/>
+      <c r="S78" s="21"/>
+      <c r="T78" s="45"/>
+      <c r="U78" s="74"/>
+      <c r="V78" s="13"/>
+    </row>
+    <row r="79" spans="1:22">
+      <c r="A79" s="31"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="34"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="42"/>
+      <c r="K79" s="42"/>
+      <c r="L79" s="42"/>
+      <c r="M79" s="42"/>
+      <c r="N79" s="42"/>
+      <c r="O79" s="21"/>
+      <c r="P79" s="21"/>
+      <c r="Q79" s="21"/>
+      <c r="R79" s="21"/>
+      <c r="S79" s="21"/>
+      <c r="T79" s="45"/>
+      <c r="U79" s="74"/>
+      <c r="V79" s="13"/>
+    </row>
+    <row r="80" spans="1:22">
+      <c r="A80" s="31"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="42"/>
+      <c r="K80" s="42"/>
+      <c r="L80" s="42"/>
+      <c r="M80" s="42"/>
+      <c r="N80" s="42"/>
+      <c r="O80" s="21"/>
+      <c r="P80" s="21"/>
+      <c r="Q80" s="21"/>
+      <c r="R80" s="21"/>
+      <c r="S80" s="21"/>
+      <c r="T80" s="45"/>
+      <c r="U80" s="74"/>
+      <c r="V80" s="13"/>
+    </row>
+    <row r="81" spans="1:22">
+      <c r="A81" s="19"/>
+      <c r="B81" s="14"/>
+      <c r="C81" s="15"/>
+      <c r="D81" s="15"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="36"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+      <c r="Q81" s="15"/>
+      <c r="R81" s="15"/>
+      <c r="S81" s="15"/>
+      <c r="T81" s="15"/>
+      <c r="U81" s="53"/>
+      <c r="V81" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -34147,7 +34583,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -34292,7 +34728,7 @@
       <c r="T2" s="9">
         <v>1.17</v>
       </c>
-      <c r="U2" s="43">
+      <c r="U2" s="38">
         <v>573730</v>
       </c>
       <c r="V2" s="10" t="s">
@@ -34346,7 +34782,7 @@
       <c r="T3">
         <v>1.27</v>
       </c>
-      <c r="U3" s="76">
+      <c r="U3" s="69">
         <v>677200</v>
       </c>
       <c r="V3" s="13" t="s">
@@ -34400,7 +34836,7 @@
       <c r="T4" s="70">
         <v>3.35</v>
       </c>
-      <c r="U4" s="76">
+      <c r="U4" s="69">
         <v>1902460</v>
       </c>
       <c r="V4" s="13" t="s">
@@ -34419,10 +34855,10 @@
       <c r="G5" s="88" t="s">
         <v>386</v>
       </c>
-      <c r="H5" s="88">
+      <c r="H5" s="108">
         <v>8.09</v>
       </c>
-      <c r="I5" s="103">
+      <c r="I5" s="108">
         <v>0.51412000000000002</v>
       </c>
       <c r="J5" s="88">
@@ -34440,25 +34876,25 @@
       <c r="N5" s="88">
         <v>8.31</v>
       </c>
-      <c r="O5" s="88">
+      <c r="O5" s="101">
         <v>1.0758000000000001</v>
       </c>
-      <c r="P5" s="88">
+      <c r="P5" s="101">
         <v>4.3499999999999997E-2</v>
       </c>
-      <c r="Q5" s="88">
+      <c r="Q5" s="101">
         <v>0.39040000000000002</v>
       </c>
-      <c r="R5" s="88">
+      <c r="R5" s="101">
         <v>0.20830000000000001</v>
       </c>
-      <c r="S5" s="88">
+      <c r="S5" s="101">
         <v>3.0099999999999998E-2</v>
       </c>
       <c r="T5" s="88">
         <v>7.48</v>
       </c>
-      <c r="U5" s="103">
+      <c r="U5" s="108">
         <v>1568520</v>
       </c>
       <c r="V5" s="84" t="s">
@@ -34512,7 +34948,7 @@
       <c r="T6" s="70">
         <v>2.46</v>
       </c>
-      <c r="U6" s="76">
+      <c r="U6" s="69">
         <v>998380</v>
       </c>
       <c r="V6" s="13" t="s">
@@ -34563,7 +34999,7 @@
       <c r="T7" s="70">
         <v>0.76</v>
       </c>
-      <c r="U7" s="76">
+      <c r="U7" s="69">
         <v>454240</v>
       </c>
       <c r="V7" s="13" t="s">
@@ -34611,7 +35047,7 @@
       <c r="T8" s="70">
         <v>1.06</v>
       </c>
-      <c r="U8" s="76">
+      <c r="U8" s="69">
         <v>3023370</v>
       </c>
       <c r="V8" s="13" t="s">
@@ -34669,7 +35105,7 @@
       <c r="T9" s="70">
         <v>1.55</v>
       </c>
-      <c r="U9" s="76">
+      <c r="U9" s="69">
         <v>1108870</v>
       </c>
       <c r="V9" s="13" t="s">
@@ -34697,7 +35133,7 @@
       <c r="R10" s="46"/>
       <c r="S10" s="21"/>
       <c r="T10" s="70"/>
-      <c r="U10" s="76"/>
+      <c r="U10" s="69"/>
       <c r="V10" s="13"/>
     </row>
     <row r="11" spans="1:22">
@@ -34723,7 +35159,7 @@
       <c r="T11" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="U11" s="53"/>
+      <c r="U11" s="39"/>
       <c r="V11" s="16"/>
     </row>
     <row r="12" spans="1:22">
@@ -34768,7 +35204,7 @@
       <c r="T12">
         <v>1.54</v>
       </c>
-      <c r="U12" s="76">
+      <c r="U12" s="69">
         <v>299950</v>
       </c>
       <c r="V12" s="13" t="s">
@@ -34787,10 +35223,10 @@
       <c r="G13" s="82" t="s">
         <v>412</v>
       </c>
-      <c r="H13" s="82">
+      <c r="H13" s="91">
         <v>30.45</v>
       </c>
-      <c r="I13" s="82">
+      <c r="I13" s="91">
         <v>0.13450000000000001</v>
       </c>
       <c r="J13" s="82">
@@ -34808,25 +35244,25 @@
       <c r="N13" s="82">
         <v>20.57</v>
       </c>
-      <c r="O13" s="82">
+      <c r="O13" s="83">
         <v>0.43080000000000002</v>
       </c>
-      <c r="P13" s="82">
+      <c r="P13" s="83">
         <v>0.60260000000000002</v>
       </c>
-      <c r="Q13" s="82">
+      <c r="Q13" s="83">
         <v>0.13450000000000001</v>
       </c>
-      <c r="R13" s="82">
+      <c r="R13" s="83">
         <v>0.1346</v>
       </c>
-      <c r="S13" s="82">
+      <c r="S13" s="83">
         <v>1.3150999999999999</v>
       </c>
       <c r="T13" s="82">
         <v>5.99</v>
       </c>
-      <c r="U13" s="100">
+      <c r="U13" s="81">
         <v>410410</v>
       </c>
       <c r="V13" s="84" t="s">
@@ -34872,7 +35308,7 @@
       <c r="T14">
         <v>1.28</v>
       </c>
-      <c r="U14" s="76">
+      <c r="U14" s="69">
         <v>625790</v>
       </c>
       <c r="V14" s="13" t="s">
@@ -34930,7 +35366,7 @@
       <c r="T15" s="35">
         <v>1.76</v>
       </c>
-      <c r="U15" s="44">
+      <c r="U15" s="24">
         <v>165780</v>
       </c>
       <c r="V15" s="13" t="s">
@@ -34958,7 +35394,7 @@
       <c r="R16" s="46"/>
       <c r="S16" s="21"/>
       <c r="T16" s="35"/>
-      <c r="U16" s="44"/>
+      <c r="U16" s="24"/>
       <c r="V16" s="13"/>
     </row>
     <row r="17" spans="1:22">
@@ -34984,7 +35420,7 @@
       <c r="T17" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="U17" s="53"/>
+      <c r="U17" s="39"/>
       <c r="V17" s="16"/>
     </row>
     <row r="18" spans="1:22">
@@ -35040,7 +35476,7 @@
       <c r="T18" s="45">
         <v>5.03</v>
       </c>
-      <c r="U18" s="74">
+      <c r="U18" s="98">
         <v>181510</v>
       </c>
       <c r="V18" s="13" t="s">

</xml_diff>

<commit_message>
Code refactoring for bit operation
</commit_message>
<xml_diff>
--- a/Stock/US_Stock.xlsx
+++ b/Stock/US_Stock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeetCode\Stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF74D9F7-F7B5-44D7-AD47-184274BE309F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56E6529-F1D7-4C4C-821A-CF6F6DA3D1DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Technology" sheetId="14" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="655">
   <si>
     <t>代码</t>
   </si>
@@ -2013,6 +2013,24 @@
   </si>
   <si>
     <t>Streaming Video</t>
+  </si>
+  <si>
+    <t>FOOT LOCKER INC</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Shoes store</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>ALTRIA GROUP INC</t>
+  </si>
+  <si>
+    <t>Ciga</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2293,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2436,6 +2454,7 @@
     <xf numFmtId="8" fontId="0" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2754,7 +2773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3B4BCA-42DA-4C85-9005-E70B6BE65D74}">
   <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection sqref="A1:XFD80"/>
     </sheetView>
   </sheetViews>
@@ -35613,10 +35632,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554D201E-890B-41A2-9456-C006731550ED}">
-  <dimension ref="A1:V64"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
-    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -36970,1397 +36989,1403 @@
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="18"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
-      <c r="S24" s="22"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="16"/>
+      <c r="B24" s="11" t="s">
+        <v>649</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="34" t="s">
+        <v>650</v>
+      </c>
+      <c r="H24" s="24">
+        <v>2.81</v>
+      </c>
+      <c r="I24" s="24">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="J24" s="12">
+        <v>6</v>
+      </c>
+      <c r="K24" s="42">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="L24" s="42">
+        <v>4.34</v>
+      </c>
+      <c r="M24" s="42">
+        <v>3.93</v>
+      </c>
+      <c r="N24" s="45">
+        <v>0.36</v>
+      </c>
+      <c r="O24" s="85">
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="P24" s="85">
+        <v>3.3E-3</v>
+      </c>
+      <c r="Q24" s="85">
+        <v>0.1116</v>
+      </c>
+      <c r="R24" s="85">
+        <v>0.1961</v>
+      </c>
+      <c r="S24" s="85">
+        <v>1.3416999999999999</v>
+      </c>
+      <c r="T24" s="45">
+        <v>1.97</v>
+      </c>
+      <c r="U24" s="98">
+        <v>156960</v>
+      </c>
+      <c r="V24" s="23" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="78"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="16"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B26" s="11" t="s">
         <v>299</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="34" t="s">
-        <v>298</v>
-      </c>
-      <c r="H25" s="24">
-        <v>193.53</v>
-      </c>
-      <c r="I25" s="24">
-        <v>8.2200000000000006</v>
-      </c>
-      <c r="J25" s="42">
-        <v>19.43</v>
-      </c>
-      <c r="K25" s="42">
-        <v>10.43</v>
-      </c>
-      <c r="L25" s="42">
-        <v>16.82</v>
-      </c>
-      <c r="M25" s="42">
-        <v>15.4</v>
-      </c>
-      <c r="N25" s="42">
-        <v>5.19</v>
-      </c>
-      <c r="O25" s="21">
-        <v>-4.1200000000000001E-2</v>
-      </c>
-      <c r="P25" s="21">
-        <v>2.6599999999999999E-2</v>
-      </c>
-      <c r="Q25" s="21">
-        <v>0.32340000000000002</v>
-      </c>
-      <c r="R25" s="21">
-        <v>0.54120000000000001</v>
-      </c>
-      <c r="S25" s="21">
-        <v>2.7753000000000001</v>
-      </c>
-      <c r="T25" s="12">
-        <v>0.84</v>
-      </c>
-      <c r="U25" s="24">
-        <v>431240</v>
-      </c>
-      <c r="V25" s="13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="18"/>
-      <c r="B26" s="86" t="s">
-        <v>427</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
-      <c r="G26" s="80" t="s">
-        <v>428</v>
-      </c>
-      <c r="H26" s="81">
-        <v>32.090000000000003</v>
-      </c>
-      <c r="I26" s="81">
-        <v>1.01</v>
-      </c>
-      <c r="J26" s="82">
-        <v>29.46</v>
-      </c>
-      <c r="K26" s="82">
-        <v>8.08</v>
-      </c>
-      <c r="L26" s="82">
-        <v>27.71</v>
-      </c>
-      <c r="M26" s="82">
-        <v>29.64</v>
-      </c>
-      <c r="N26" s="82">
-        <v>7.71</v>
-      </c>
-      <c r="O26" s="83">
-        <v>0.1125</v>
-      </c>
-      <c r="P26" s="83">
-        <v>0.18090000000000001</v>
-      </c>
-      <c r="Q26" s="83">
-        <v>0.35210000000000002</v>
-      </c>
-      <c r="R26" s="83">
-        <v>0.27629999999999999</v>
-      </c>
-      <c r="S26" s="83">
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="T26" s="82">
-        <v>3.29</v>
-      </c>
-      <c r="U26" s="81">
-        <v>1190370</v>
-      </c>
-      <c r="V26" s="84" t="s">
-        <v>429</v>
+      <c r="G26" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="H26" s="24">
+        <v>193.53</v>
+      </c>
+      <c r="I26" s="24">
+        <v>8.2200000000000006</v>
+      </c>
+      <c r="J26" s="42">
+        <v>19.43</v>
+      </c>
+      <c r="K26" s="42">
+        <v>10.43</v>
+      </c>
+      <c r="L26" s="42">
+        <v>16.82</v>
+      </c>
+      <c r="M26" s="42">
+        <v>15.4</v>
+      </c>
+      <c r="N26" s="42">
+        <v>5.19</v>
+      </c>
+      <c r="O26" s="21">
+        <v>-4.1200000000000001E-2</v>
+      </c>
+      <c r="P26" s="21">
+        <v>2.6599999999999999E-2</v>
+      </c>
+      <c r="Q26" s="21">
+        <v>0.32340000000000002</v>
+      </c>
+      <c r="R26" s="21">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="S26" s="21">
+        <v>2.7753000000000001</v>
+      </c>
+      <c r="T26" s="12">
+        <v>0.84</v>
+      </c>
+      <c r="U26" s="24">
+        <v>431240</v>
+      </c>
+      <c r="V26" s="13" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="27" spans="1:22">
       <c r="A27" s="18"/>
-      <c r="B27" s="11" t="s">
-        <v>503</v>
+      <c r="B27" s="86" t="s">
+        <v>427</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
-      <c r="G27" s="34" t="s">
-        <v>504</v>
-      </c>
-      <c r="H27" s="24">
-        <v>27.59</v>
-      </c>
-      <c r="I27" s="24">
-        <v>1.34</v>
-      </c>
-      <c r="J27" s="42">
-        <v>25.05</v>
-      </c>
-      <c r="K27" s="42">
-        <v>16.2</v>
-      </c>
-      <c r="L27" s="42">
-        <v>19.690000000000001</v>
-      </c>
-      <c r="M27" s="42">
-        <v>20.18</v>
-      </c>
-      <c r="N27" s="42">
-        <v>3.46</v>
-      </c>
-      <c r="O27" s="21">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="P27" s="21">
-        <v>6.4600000000000005E-2</v>
-      </c>
-      <c r="Q27" s="21">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="R27" s="21">
-        <v>0.65300000000000002</v>
-      </c>
-      <c r="S27" s="21">
-        <v>3.1659000000000002</v>
-      </c>
-      <c r="T27" s="35">
-        <v>0.92</v>
-      </c>
-      <c r="U27" s="24">
-        <v>496100</v>
-      </c>
-      <c r="V27" s="13" t="s">
-        <v>505</v>
+      <c r="G27" s="80" t="s">
+        <v>428</v>
+      </c>
+      <c r="H27" s="81">
+        <v>32.090000000000003</v>
+      </c>
+      <c r="I27" s="81">
+        <v>1.01</v>
+      </c>
+      <c r="J27" s="82">
+        <v>29.46</v>
+      </c>
+      <c r="K27" s="82">
+        <v>8.08</v>
+      </c>
+      <c r="L27" s="82">
+        <v>27.71</v>
+      </c>
+      <c r="M27" s="82">
+        <v>29.64</v>
+      </c>
+      <c r="N27" s="82">
+        <v>7.71</v>
+      </c>
+      <c r="O27" s="83">
+        <v>0.1125</v>
+      </c>
+      <c r="P27" s="83">
+        <v>0.18090000000000001</v>
+      </c>
+      <c r="Q27" s="83">
+        <v>0.35210000000000002</v>
+      </c>
+      <c r="R27" s="83">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="S27" s="83">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="T27" s="82">
+        <v>3.29</v>
+      </c>
+      <c r="U27" s="81">
+        <v>1190370</v>
+      </c>
+      <c r="V27" s="84" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="28" spans="1:22">
       <c r="A28" s="18"/>
       <c r="B28" s="11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="34" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="H28" s="24">
-        <v>87.76</v>
+        <v>27.59</v>
       </c>
       <c r="I28" s="24">
-        <v>8.2200000000000006</v>
+        <v>1.34</v>
       </c>
       <c r="J28" s="42">
-        <v>10.16</v>
+        <v>25.05</v>
       </c>
       <c r="K28" s="42">
-        <v>1.2</v>
+        <v>16.2</v>
       </c>
       <c r="L28" s="42">
-        <v>6.63</v>
+        <v>19.690000000000001</v>
       </c>
       <c r="M28" s="42">
-        <v>4.9000000000000004</v>
+        <v>20.18</v>
       </c>
       <c r="N28" s="42">
-        <v>1.68</v>
+        <v>3.46</v>
       </c>
       <c r="O28" s="21">
-        <v>2.1399999999999999E-2</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="P28" s="21">
-        <v>1.29E-2</v>
-      </c>
-      <c r="Q28" s="21"/>
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="Q28" s="21">
+        <v>0.24399999999999999</v>
+      </c>
       <c r="R28" s="21">
-        <v>0.11990000000000001</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="S28" s="21">
-        <v>1.3608</v>
+        <v>3.1659000000000002</v>
       </c>
       <c r="T28" s="35">
-        <v>0.68</v>
+        <v>0.92</v>
       </c>
       <c r="U28" s="24">
-        <v>304390</v>
+        <v>496100</v>
       </c>
       <c r="V28" s="13" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" spans="1:22">
       <c r="A29" s="18"/>
       <c r="B29" s="11" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
       <c r="G29" s="34" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="H29" s="24">
-        <v>58.7</v>
+        <v>87.76</v>
       </c>
       <c r="I29" s="24">
-        <v>2.95</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="J29" s="42">
-        <v>23.39</v>
-      </c>
-      <c r="K29" s="42"/>
+        <v>10.16</v>
+      </c>
+      <c r="K29" s="42">
+        <v>1.2</v>
+      </c>
       <c r="L29" s="42">
-        <v>19.27</v>
+        <v>6.63</v>
       </c>
       <c r="M29" s="42">
-        <v>17.3</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N29" s="42">
-        <v>3.69</v>
+        <v>1.68</v>
       </c>
       <c r="O29" s="21">
-        <v>-1.9E-2</v>
+        <v>2.1399999999999999E-2</v>
       </c>
       <c r="P29" s="21">
-        <v>1.9400000000000001E-2</v>
-      </c>
-      <c r="Q29" s="21">
-        <v>0.27689999999999998</v>
-      </c>
+        <v>1.29E-2</v>
+      </c>
+      <c r="Q29" s="21"/>
       <c r="R29" s="21">
-        <v>-15.1244</v>
+        <v>0.11990000000000001</v>
       </c>
       <c r="S29" s="21">
-        <v>72.504300000000001</v>
+        <v>1.3608</v>
       </c>
       <c r="T29" s="35">
-        <v>1.06</v>
+        <v>0.68</v>
       </c>
       <c r="U29" s="24">
-        <v>457520</v>
+        <v>304390</v>
       </c>
       <c r="V29" s="13" t="s">
-        <v>539</v>
+        <v>508</v>
       </c>
     </row>
     <row r="30" spans="1:22">
       <c r="A30" s="18"/>
       <c r="B30" s="11" t="s">
-        <v>537</v>
+        <v>509</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
       <c r="F30" s="12"/>
       <c r="G30" s="34" t="s">
-        <v>536</v>
+        <v>510</v>
       </c>
       <c r="H30" s="24">
-        <v>36.090000000000003</v>
+        <v>58.7</v>
       </c>
       <c r="I30" s="24">
-        <v>2.5</v>
+        <v>2.95</v>
       </c>
       <c r="J30" s="42">
-        <v>17.12</v>
-      </c>
-      <c r="K30" s="42">
-        <v>4.84</v>
-      </c>
+        <v>23.39</v>
+      </c>
+      <c r="K30" s="42"/>
       <c r="L30" s="42">
-        <v>13.15</v>
+        <v>19.27</v>
       </c>
       <c r="M30" s="42">
-        <v>14.97</v>
+        <v>17.3</v>
       </c>
       <c r="N30" s="42">
-        <v>2.15</v>
+        <v>3.69</v>
       </c>
       <c r="O30" s="21">
-        <v>-1.1900000000000001E-2</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="P30" s="21">
-        <v>-3.0999999999999999E-3</v>
+        <v>1.9400000000000001E-2</v>
       </c>
       <c r="Q30" s="21">
-        <v>0.20899999999999999</v>
+        <v>0.27689999999999998</v>
       </c>
       <c r="R30" s="21">
-        <v>0.28610000000000002</v>
+        <v>-15.1244</v>
       </c>
       <c r="S30" s="21">
-        <v>1.8532</v>
+        <v>72.504300000000001</v>
       </c>
       <c r="T30" s="35">
-        <v>0.61</v>
+        <v>1.06</v>
       </c>
       <c r="U30" s="24">
-        <v>419130</v>
+        <v>457520</v>
       </c>
       <c r="V30" s="13" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="18"/>
       <c r="B31" s="11" t="s">
-        <v>528</v>
+        <v>537</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="12"/>
       <c r="F31" s="12"/>
       <c r="G31" s="34" t="s">
-        <v>527</v>
+        <v>536</v>
       </c>
       <c r="H31" s="24">
-        <v>22.15</v>
+        <v>36.090000000000003</v>
       </c>
       <c r="I31" s="24">
-        <v>0.94699999999999995</v>
+        <v>2.5</v>
       </c>
       <c r="J31" s="42">
-        <v>21.69</v>
+        <v>17.12</v>
       </c>
       <c r="K31" s="42">
-        <v>8.1999999999999993</v>
+        <v>4.84</v>
       </c>
       <c r="L31" s="42">
-        <v>14.74</v>
+        <v>13.15</v>
       </c>
       <c r="M31" s="42">
-        <v>11.94</v>
+        <v>14.97</v>
       </c>
       <c r="N31" s="42">
-        <v>1.64</v>
+        <v>2.15</v>
       </c>
       <c r="O31" s="21">
-        <v>-1.4200000000000001E-2</v>
+        <v>-1.1900000000000001E-2</v>
       </c>
       <c r="P31" s="21">
-        <v>4.9299999999999997E-2</v>
+        <v>-3.0999999999999999E-3</v>
       </c>
       <c r="Q31" s="21">
-        <v>0.16900000000000001</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="R31" s="21">
-        <v>0.37969999999999998</v>
+        <v>0.28610000000000002</v>
       </c>
       <c r="S31" s="21">
-        <v>3.3776999999999999</v>
+        <v>1.8532</v>
       </c>
       <c r="T31" s="35">
-        <v>0.75</v>
+        <v>0.61</v>
       </c>
       <c r="U31" s="24">
-        <v>434450</v>
+        <v>419130</v>
       </c>
       <c r="V31" s="13" t="s">
-        <v>529</v>
+        <v>538</v>
       </c>
     </row>
     <row r="32" spans="1:22">
       <c r="A32" s="18"/>
       <c r="B32" s="11" t="s">
-        <v>540</v>
+        <v>528</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
       <c r="G32" s="34" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="H32" s="24">
-        <v>15.22</v>
+        <v>22.15</v>
       </c>
       <c r="I32" s="24">
-        <v>0.86199999999999999</v>
+        <v>0.94699999999999995</v>
       </c>
       <c r="J32" s="42">
-        <v>33.380000000000003</v>
+        <v>21.69</v>
       </c>
       <c r="K32" s="42">
-        <v>10.029999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="L32" s="42">
-        <v>24.59</v>
+        <v>14.74</v>
       </c>
       <c r="M32" s="42">
-        <v>15.22</v>
+        <v>11.94</v>
       </c>
       <c r="N32" s="42">
-        <v>1.88</v>
+        <v>1.64</v>
       </c>
       <c r="O32" s="21">
-        <v>-3.8999999999999998E-3</v>
+        <v>-1.4200000000000001E-2</v>
       </c>
       <c r="P32" s="21">
-        <v>-4.2900000000000001E-2</v>
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="Q32" s="21">
+        <v>0.16900000000000001</v>
       </c>
       <c r="R32" s="21">
-        <v>0.30209999999999998</v>
+        <v>0.37969999999999998</v>
       </c>
       <c r="S32" s="21">
-        <v>2.4394999999999998</v>
+        <v>3.3776999999999999</v>
       </c>
       <c r="T32" s="35">
-        <v>0.6</v>
+        <v>0.75</v>
       </c>
       <c r="U32" s="24">
-        <v>425160</v>
+        <v>434450</v>
       </c>
       <c r="V32" s="13" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="18"/>
       <c r="B33" s="11" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="34" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="H33" s="24">
-        <v>25.04</v>
+        <v>15.22</v>
       </c>
       <c r="I33" s="24">
-        <v>0.61129999999999995</v>
+        <v>0.86199999999999999</v>
       </c>
       <c r="J33" s="42">
-        <v>25.75</v>
+        <v>33.380000000000003</v>
       </c>
       <c r="K33" s="42">
-        <v>4.1900000000000004</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="L33" s="42">
-        <v>21.61</v>
+        <v>24.59</v>
       </c>
       <c r="M33" s="42">
-        <v>21.43</v>
+        <v>15.22</v>
       </c>
       <c r="N33" s="42">
-        <v>2.62</v>
+        <v>1.88</v>
       </c>
       <c r="O33" s="21">
-        <v>3.8999999999999998E-3</v>
+        <v>-3.8999999999999998E-3</v>
       </c>
       <c r="P33" s="21">
-        <v>9.3200000000000005E-2</v>
-      </c>
-      <c r="Q33" s="46">
-        <v>0.1358</v>
+        <v>-4.2900000000000001E-2</v>
       </c>
       <c r="R33" s="21">
-        <v>0.1648</v>
+        <v>0.30209999999999998</v>
       </c>
       <c r="S33" s="21">
-        <v>6.2300000000000001E-2</v>
+        <v>2.4394999999999998</v>
       </c>
       <c r="T33" s="35">
-        <v>2.1800000000000002</v>
+        <v>0.6</v>
       </c>
       <c r="U33" s="24">
-        <v>506460</v>
+        <v>425160</v>
       </c>
       <c r="V33" s="13" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="34" spans="1:22">
       <c r="A34" s="18"/>
-      <c r="B34" s="86" t="s">
+      <c r="B34" s="11" t="s">
+        <v>543</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="34" t="s">
+        <v>544</v>
+      </c>
+      <c r="H34" s="24">
+        <v>25.04</v>
+      </c>
+      <c r="I34" s="24">
+        <v>0.61129999999999995</v>
+      </c>
+      <c r="J34" s="42">
+        <v>25.75</v>
+      </c>
+      <c r="K34" s="42">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="L34" s="42">
+        <v>21.61</v>
+      </c>
+      <c r="M34" s="42">
+        <v>21.43</v>
+      </c>
+      <c r="N34" s="42">
+        <v>2.62</v>
+      </c>
+      <c r="O34" s="21">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="P34" s="21">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="Q34" s="46">
+        <v>0.1358</v>
+      </c>
+      <c r="R34" s="21">
+        <v>0.1648</v>
+      </c>
+      <c r="S34" s="21">
+        <v>6.2300000000000001E-2</v>
+      </c>
+      <c r="T34" s="35">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="U34" s="24">
+        <v>506460</v>
+      </c>
+      <c r="V34" s="13" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" s="18"/>
+      <c r="B35" s="60" t="s">
         <v>530</v>
       </c>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="82"/>
-      <c r="G34" s="80" t="s">
+      <c r="C35" s="42"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="71" t="s">
         <v>531</v>
       </c>
-      <c r="H34" s="81">
+      <c r="H35" s="98">
         <v>35.869999999999997</v>
       </c>
-      <c r="I34" s="81">
+      <c r="I35" s="98">
         <v>2.81</v>
       </c>
-      <c r="J34" s="82">
+      <c r="J35" s="42">
         <v>18.71</v>
       </c>
-      <c r="K34" s="82">
+      <c r="K35" s="42">
         <v>0.7</v>
       </c>
-      <c r="L34" s="82">
+      <c r="L35" s="42">
         <v>12.34</v>
       </c>
-      <c r="M34" s="82">
+      <c r="M35" s="42">
         <v>14.44</v>
       </c>
-      <c r="N34" s="82">
+      <c r="N35" s="42">
         <v>1.42</v>
       </c>
-      <c r="O34" s="83">
+      <c r="O35" s="85">
         <v>0.1799</v>
       </c>
-      <c r="P34" s="83">
+      <c r="P35" s="85">
         <v>0.19939999999999999</v>
       </c>
-      <c r="Q34" s="83">
+      <c r="Q35" s="85">
         <v>0.23300000000000001</v>
       </c>
-      <c r="R34" s="83">
+      <c r="R35" s="85">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="S34" s="83">
+      <c r="S35" s="85">
         <v>0.64259999999999995</v>
       </c>
-      <c r="T34" s="87">
+      <c r="T35" s="45">
         <v>1.1599999999999999</v>
       </c>
-      <c r="U34" s="81">
+      <c r="U35" s="98">
         <v>680410</v>
       </c>
-      <c r="V34" s="84" t="s">
+      <c r="V35" s="23" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="35" spans="1:22">
-      <c r="A35" s="19"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="22"/>
-      <c r="R35" s="22"/>
-      <c r="S35" s="22"/>
-      <c r="T35" s="37"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="16"/>
-    </row>
     <row r="36" spans="1:22">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22"/>
+      <c r="S36" s="22"/>
+      <c r="T36" s="37"/>
+      <c r="U36" s="15"/>
+      <c r="V36" s="16"/>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37" s="17" t="s">
         <v>502</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B37" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="28" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="28" t="s">
         <v>268</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H37" s="38">
         <v>88.26</v>
       </c>
-      <c r="I36" s="38">
+      <c r="I37" s="38">
         <v>2.73</v>
       </c>
-      <c r="J36" s="9">
+      <c r="J37" s="9">
         <v>24.56</v>
       </c>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9">
+      <c r="K37" s="9"/>
+      <c r="L37" s="9">
         <v>17.53</v>
       </c>
-      <c r="M36" s="9">
+      <c r="M37" s="9">
         <v>17.84</v>
       </c>
-      <c r="N36" s="9">
+      <c r="N37" s="9">
         <v>3.33</v>
       </c>
-      <c r="O36" s="20">
+      <c r="O37" s="20">
         <v>0.1002</v>
       </c>
-      <c r="P36" s="20">
+      <c r="P37" s="20">
         <v>0.1237</v>
       </c>
-      <c r="Q36" s="20">
+      <c r="Q37" s="20">
         <v>0.20330000000000001</v>
       </c>
-      <c r="R36" s="20">
+      <c r="R37" s="20">
         <v>-0.66659999999999997</v>
       </c>
-      <c r="S36" s="20">
+      <c r="S37" s="20">
         <v>-3.0518999999999998</v>
       </c>
-      <c r="T36" s="9">
+      <c r="T37" s="9">
         <v>0.93</v>
       </c>
-      <c r="U36" s="38">
+      <c r="U37" s="38">
         <v>77060</v>
       </c>
-      <c r="V36" s="10" t="s">
+      <c r="V37" s="10" t="s">
         <v>269</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37" s="18"/>
-      <c r="B37" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="34" t="s">
-        <v>270</v>
-      </c>
-      <c r="H37" s="24">
-        <v>135.86000000000001</v>
-      </c>
-      <c r="I37" s="24">
-        <v>5.73</v>
-      </c>
-      <c r="J37" s="12">
-        <v>23.1</v>
-      </c>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12">
-        <v>18</v>
-      </c>
-      <c r="M37" s="42">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="N37" s="12">
-        <v>6.53</v>
-      </c>
-      <c r="O37" s="21">
-        <v>-5.1400000000000001E-2</v>
-      </c>
-      <c r="P37" s="21">
-        <v>3.3300000000000003E-2</v>
-      </c>
-      <c r="Q37" s="21">
-        <v>0.49840000000000001</v>
-      </c>
-      <c r="R37" s="21">
-        <v>-0.79890000000000005</v>
-      </c>
-      <c r="S37" s="21">
-        <v>-5.7922000000000002</v>
-      </c>
-      <c r="T37" s="12">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="U37" s="44">
-        <v>102810</v>
-      </c>
-      <c r="V37" s="13" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="38" spans="1:22">
       <c r="A38" s="18"/>
       <c r="B38" s="11" t="s">
-        <v>273</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
       <c r="G38" s="34" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="H38" s="24">
-        <v>13.77</v>
+        <v>135.86000000000001</v>
       </c>
       <c r="I38" s="24">
-        <v>1.41</v>
+        <v>5.73</v>
       </c>
       <c r="J38" s="12">
-        <v>19.489999999999998</v>
-      </c>
-      <c r="K38" s="12">
-        <v>6.05</v>
-      </c>
+        <v>23.1</v>
+      </c>
+      <c r="K38" s="12"/>
       <c r="L38" s="12">
-        <v>15.42</v>
+        <v>18</v>
       </c>
       <c r="M38" s="42">
-        <v>16.32</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="N38" s="12">
-        <v>2.2799999999999998</v>
+        <v>6.53</v>
       </c>
       <c r="O38" s="21">
-        <v>0.36159999999999998</v>
+        <v>-5.1400000000000001E-2</v>
       </c>
       <c r="P38" s="21">
-        <v>0.27200000000000002</v>
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="Q38" s="21">
-        <v>0.39410000000000001</v>
+        <v>0.49840000000000001</v>
       </c>
       <c r="R38" s="21">
-        <v>0.30499999999999999</v>
+        <v>-0.79890000000000005</v>
       </c>
       <c r="S38" s="21">
-        <v>5.3666999999999998</v>
+        <v>-5.7922000000000002</v>
       </c>
       <c r="T38" s="12">
-        <v>1.17</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="U38" s="44">
-        <v>889370</v>
+        <v>102810</v>
       </c>
       <c r="V38" s="13" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="1:22">
       <c r="A39" s="18"/>
       <c r="B39" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
+        <v>273</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="G39" s="34" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="H39" s="24">
-        <v>14.39</v>
+        <v>13.77</v>
       </c>
       <c r="I39" s="24">
-        <v>0.41138999999999998</v>
+        <v>1.41</v>
       </c>
       <c r="J39" s="12">
-        <v>38.67</v>
-      </c>
-      <c r="K39" s="12"/>
+        <v>19.489999999999998</v>
+      </c>
+      <c r="K39" s="12">
+        <v>6.05</v>
+      </c>
       <c r="L39" s="12">
-        <v>32.53</v>
+        <v>15.42</v>
       </c>
       <c r="M39" s="42">
-        <v>24.26</v>
+        <v>16.32</v>
       </c>
       <c r="N39" s="12">
-        <v>4.1399999999999997</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="O39" s="21">
-        <v>0.12659999999999999</v>
+        <v>0.36159999999999998</v>
       </c>
       <c r="P39" s="21">
-        <v>0.1835</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="Q39" s="21">
-        <v>0.19059999999999999</v>
+        <v>0.39410000000000001</v>
       </c>
       <c r="R39" s="21">
-        <v>-0.13100000000000001</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="S39" s="21">
-        <v>-1.2737000000000001</v>
+        <v>5.3666999999999998</v>
       </c>
       <c r="T39" s="12">
-        <v>1.55</v>
+        <v>1.17</v>
       </c>
       <c r="U39" s="44">
-        <v>279080</v>
+        <v>889370</v>
       </c>
       <c r="V39" s="13" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:22">
       <c r="A40" s="18"/>
       <c r="B40" s="11" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
       <c r="F40" s="12"/>
       <c r="G40" s="34" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H40" s="24">
-        <v>24.12</v>
+        <v>14.39</v>
       </c>
       <c r="I40" s="24">
-        <v>0.37378</v>
-      </c>
-      <c r="J40" s="42">
-        <v>72.61</v>
-      </c>
-      <c r="K40" s="12">
-        <v>14.78</v>
-      </c>
-      <c r="L40" s="42">
-        <v>43.33</v>
+        <v>0.41138999999999998</v>
+      </c>
+      <c r="J40" s="12">
+        <v>38.67</v>
+      </c>
+      <c r="K40" s="12"/>
+      <c r="L40" s="12">
+        <v>32.53</v>
       </c>
       <c r="M40" s="42">
-        <v>44.74</v>
-      </c>
-      <c r="N40" s="42">
-        <v>4.2300000000000004</v>
+        <v>24.26</v>
+      </c>
+      <c r="N40" s="12">
+        <v>4.1399999999999997</v>
       </c>
       <c r="O40" s="21">
-        <v>6.3399999999999998E-2</v>
+        <v>0.12659999999999999</v>
       </c>
       <c r="P40" s="21">
-        <v>2.5000000000000001E-3</v>
+        <v>0.1835</v>
       </c>
       <c r="Q40" s="21">
-        <v>0.1207</v>
+        <v>0.19059999999999999</v>
       </c>
       <c r="R40" s="21">
-        <v>0.20780000000000001</v>
+        <v>-0.13100000000000001</v>
       </c>
       <c r="S40" s="21">
-        <v>1.7602</v>
+        <v>-1.2737000000000001</v>
       </c>
       <c r="T40" s="12">
-        <v>1.56</v>
+        <v>1.55</v>
       </c>
       <c r="U40" s="44">
-        <v>68540</v>
+        <v>279080</v>
       </c>
       <c r="V40" s="13" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:22">
       <c r="A41" s="18"/>
       <c r="B41" s="11" t="s">
-        <v>547</v>
+        <v>279</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
       <c r="G41" s="34" t="s">
-        <v>546</v>
+        <v>280</v>
       </c>
       <c r="H41" s="24">
-        <v>5.14</v>
+        <v>24.12</v>
       </c>
       <c r="I41" s="24">
-        <v>0.26096999999999998</v>
+        <v>0.37378</v>
       </c>
       <c r="J41" s="42">
-        <v>21.46</v>
-      </c>
-      <c r="K41" s="42"/>
+        <v>72.61</v>
+      </c>
+      <c r="K41" s="12">
+        <v>14.78</v>
+      </c>
       <c r="L41" s="42">
-        <v>18.399999999999999</v>
+        <v>43.33</v>
       </c>
       <c r="M41" s="42">
-        <v>19.22</v>
+        <v>44.74</v>
       </c>
       <c r="N41" s="42">
-        <v>3.75</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="O41" s="21">
-        <v>0.1285</v>
+        <v>6.3399999999999998E-2</v>
       </c>
       <c r="P41" s="21">
-        <v>4.6800000000000001E-2</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="Q41" s="21">
-        <v>0.34279999999999999</v>
+        <v>0.1207</v>
       </c>
       <c r="R41" s="21">
-        <v>-0.37859999999999999</v>
+        <v>0.20780000000000001</v>
       </c>
       <c r="S41" s="21">
-        <v>-5.4268999999999998</v>
-      </c>
-      <c r="T41" s="35">
-        <v>1.58</v>
+        <v>1.7602</v>
+      </c>
+      <c r="T41" s="12">
+        <v>1.56</v>
       </c>
       <c r="U41" s="44">
-        <v>1230010</v>
+        <v>68540</v>
       </c>
       <c r="V41" s="13" t="s">
-        <v>548</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42" spans="1:22">
       <c r="A42" s="18"/>
       <c r="B42" s="11" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
       <c r="G42" s="34" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="H42" s="24">
-        <v>4.38</v>
+        <v>5.14</v>
       </c>
       <c r="I42" s="24">
-        <v>0.21448</v>
+        <v>0.26096999999999998</v>
       </c>
       <c r="J42" s="42">
-        <v>32.979999999999997</v>
-      </c>
-      <c r="K42" s="42">
-        <v>7.27</v>
-      </c>
+        <v>21.46</v>
+      </c>
+      <c r="K42" s="42"/>
       <c r="L42" s="42">
-        <v>16.61</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="M42" s="42">
-        <v>18.16</v>
+        <v>19.22</v>
       </c>
       <c r="N42" s="42">
-        <v>2.61</v>
+        <v>3.75</v>
       </c>
       <c r="O42" s="21">
-        <v>-3.6799999999999999E-2</v>
+        <v>0.1285</v>
       </c>
       <c r="P42" s="21">
-        <v>-8.8000000000000005E-3</v>
+        <v>4.6800000000000001E-2</v>
       </c>
       <c r="Q42" s="21">
-        <v>0.23230000000000001</v>
+        <v>0.34279999999999999</v>
       </c>
       <c r="R42" s="21">
-        <v>0.22309999999999999</v>
+        <v>-0.37859999999999999</v>
       </c>
       <c r="S42" s="21">
-        <v>7.1920000000000002</v>
+        <v>-5.4268999999999998</v>
       </c>
       <c r="T42" s="35">
-        <v>1.9</v>
+        <v>1.58</v>
       </c>
       <c r="U42" s="44">
-        <v>128500</v>
+        <v>1230010</v>
       </c>
       <c r="V42" s="13" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="43" spans="1:22">
       <c r="A43" s="18"/>
       <c r="B43" s="11" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
       <c r="F43" s="12"/>
       <c r="G43" s="34" t="s">
+        <v>550</v>
+      </c>
+      <c r="H43" s="24">
+        <v>4.38</v>
+      </c>
+      <c r="I43" s="24">
+        <v>0.21448</v>
+      </c>
+      <c r="J43" s="42">
+        <v>32.979999999999997</v>
+      </c>
+      <c r="K43" s="42">
+        <v>7.27</v>
+      </c>
+      <c r="L43" s="42">
+        <v>16.61</v>
+      </c>
+      <c r="M43" s="42">
+        <v>18.16</v>
+      </c>
+      <c r="N43" s="42">
+        <v>2.61</v>
+      </c>
+      <c r="O43" s="21">
+        <v>-3.6799999999999999E-2</v>
+      </c>
+      <c r="P43" s="21">
+        <v>-8.8000000000000005E-3</v>
+      </c>
+      <c r="Q43" s="21">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="R43" s="21">
+        <v>0.22309999999999999</v>
+      </c>
+      <c r="S43" s="21">
+        <v>7.1920000000000002</v>
+      </c>
+      <c r="T43" s="35">
+        <v>1.9</v>
+      </c>
+      <c r="U43" s="44">
+        <v>128500</v>
+      </c>
+      <c r="V43" s="13" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" s="18"/>
+      <c r="B44" s="11" t="s">
+        <v>556</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="34" t="s">
         <v>557</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H44" s="24">
         <v>25.23</v>
       </c>
-      <c r="I43" s="24">
+      <c r="I44" s="24">
         <v>1.07</v>
       </c>
-      <c r="J43" s="42">
+      <c r="J44" s="42">
         <v>23.41</v>
       </c>
-      <c r="K43" s="12"/>
-      <c r="L43" s="42">
+      <c r="K44" s="12"/>
+      <c r="L44" s="42">
         <v>20.61</v>
       </c>
-      <c r="M43" s="42">
+      <c r="M44" s="42">
         <v>57.33</v>
       </c>
-      <c r="N43" s="42">
+      <c r="N44" s="42">
         <v>4.51</v>
       </c>
-      <c r="O43" s="21">
+      <c r="O44" s="21">
         <v>-0.15870000000000001</v>
       </c>
-      <c r="P43" s="21">
+      <c r="P44" s="21">
         <v>-3.8899999999999997E-2</v>
       </c>
-      <c r="Q43" s="21">
+      <c r="Q44" s="21">
         <v>0.3619</v>
       </c>
-      <c r="R43" s="21">
+      <c r="R44" s="21">
         <v>-0.13789999999999999</v>
       </c>
-      <c r="S43" s="21">
+      <c r="S44" s="21">
         <v>-1.3982000000000001</v>
       </c>
-      <c r="T43" s="35">
+      <c r="T44" s="35">
         <v>1.19</v>
       </c>
-      <c r="U43" s="44">
+      <c r="U44" s="44">
         <v>164880</v>
       </c>
-      <c r="V43" s="13" t="s">
+      <c r="V44" s="13" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="44" spans="1:22">
-      <c r="A44" s="19"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="22"/>
-      <c r="Q44" s="22"/>
-      <c r="R44" s="22"/>
-      <c r="S44" s="22"/>
-      <c r="T44" s="37"/>
-      <c r="U44" s="53"/>
-      <c r="V44" s="16"/>
-    </row>
     <row r="45" spans="1:22">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="19"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+      <c r="M45" s="15"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="22"/>
+      <c r="P45" s="22"/>
+      <c r="Q45" s="22"/>
+      <c r="R45" s="22"/>
+      <c r="S45" s="22"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="16"/>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" s="17" t="s">
         <v>552</v>
       </c>
-      <c r="B45" s="88" t="s">
+      <c r="B46" s="88" t="s">
         <v>293</v>
       </c>
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="88"/>
-      <c r="F45" s="88"/>
-      <c r="G45" s="88" t="s">
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
+      <c r="F46" s="88"/>
+      <c r="G46" s="88" t="s">
         <v>290</v>
       </c>
-      <c r="H45" s="88">
+      <c r="H46" s="88">
         <v>4.55</v>
       </c>
-      <c r="I45" s="88">
+      <c r="I46" s="88">
         <v>0.16194</v>
       </c>
-      <c r="J45" s="88">
+      <c r="J46" s="88">
         <v>13.93</v>
       </c>
-      <c r="K45" s="88">
+      <c r="K46" s="88">
         <v>2.62</v>
       </c>
-      <c r="L45" s="88">
+      <c r="L46" s="88">
         <v>13.8</v>
       </c>
-      <c r="M45" s="88">
+      <c r="M46" s="88">
         <v>9.9700000000000006</v>
       </c>
-      <c r="N45" s="88">
+      <c r="N46" s="88">
         <v>1.49</v>
       </c>
-      <c r="O45" s="88">
+      <c r="O46" s="88">
         <v>7.7299999999999994E-2</v>
       </c>
-      <c r="P45" s="88">
+      <c r="P46" s="88">
         <v>0.15340000000000001</v>
       </c>
-      <c r="Q45" s="88">
+      <c r="Q46" s="88">
         <v>0.20330000000000001</v>
       </c>
-      <c r="R45" s="88">
+      <c r="R46" s="88">
         <v>0.18959999999999999</v>
       </c>
-      <c r="S45" s="88">
+      <c r="S46" s="88">
         <v>0.23549999999999999</v>
       </c>
-      <c r="T45" s="88">
+      <c r="T46" s="88">
         <v>3.06</v>
       </c>
-      <c r="U45" s="88">
+      <c r="U46" s="88">
         <v>343590</v>
       </c>
-      <c r="V45" s="89" t="s">
+      <c r="V46" s="89" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="A46" s="18"/>
-      <c r="B46" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="34" t="s">
-        <v>291</v>
-      </c>
-      <c r="H46" s="24">
-        <v>135.83000000000001</v>
-      </c>
-      <c r="I46" s="24">
-        <v>3.43</v>
-      </c>
-      <c r="J46" s="12">
-        <v>32.229999999999997</v>
-      </c>
-      <c r="K46" s="12">
-        <v>14.88</v>
-      </c>
-      <c r="L46" s="12">
-        <v>27.21</v>
-      </c>
-      <c r="M46" s="42">
-        <v>33.39</v>
-      </c>
-      <c r="N46" s="12">
-        <v>3.3</v>
-      </c>
-      <c r="O46" s="21">
-        <v>7.0699999999999999E-2</v>
-      </c>
-      <c r="P46" s="21">
-        <v>8.0699999999999994E-2</v>
-      </c>
-      <c r="Q46" s="21">
-        <v>0.14219999999999999</v>
-      </c>
-      <c r="R46" s="21">
-        <v>0.47139999999999999</v>
-      </c>
-      <c r="S46" s="21">
-        <v>0.7359</v>
-      </c>
-      <c r="T46" s="35">
-        <v>2</v>
-      </c>
-      <c r="U46" s="44"/>
-      <c r="V46" s="13" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="47" spans="1:22">
       <c r="A47" s="18"/>
       <c r="B47" s="11" t="s">
-        <v>297</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
       <c r="G47" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H47" s="24">
-        <v>27.59</v>
+        <v>135.83000000000001</v>
       </c>
       <c r="I47" s="24">
-        <v>0.38627</v>
+        <v>3.43</v>
       </c>
       <c r="J47" s="12">
-        <v>42.84</v>
+        <v>32.229999999999997</v>
       </c>
       <c r="K47" s="12">
-        <v>17.04</v>
+        <v>14.88</v>
       </c>
       <c r="L47" s="12">
-        <v>34.15</v>
+        <v>27.21</v>
       </c>
       <c r="M47" s="42">
-        <v>19.96</v>
+        <v>33.39</v>
       </c>
       <c r="N47" s="12">
-        <v>6.93</v>
+        <v>3.3</v>
       </c>
       <c r="O47" s="21">
-        <v>0.17230000000000001</v>
+        <v>7.0699999999999999E-2</v>
       </c>
       <c r="P47" s="21">
-        <v>0.22109999999999999</v>
+        <v>8.0699999999999994E-2</v>
       </c>
       <c r="Q47" s="21">
-        <v>0.2641</v>
+        <v>0.14219999999999999</v>
       </c>
       <c r="R47" s="21">
-        <v>0.39879999999999999</v>
+        <v>0.47139999999999999</v>
       </c>
       <c r="S47" s="21">
-        <v>0.379</v>
+        <v>0.7359</v>
       </c>
       <c r="T47" s="35">
-        <v>2.56</v>
+        <v>2</v>
       </c>
       <c r="U47" s="44"/>
       <c r="V47" s="13" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:22">
       <c r="A48" s="18"/>
       <c r="B48" s="11" t="s">
-        <v>334</v>
-      </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
+        <v>297</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="G48" s="34" t="s">
-        <v>333</v>
+        <v>292</v>
       </c>
       <c r="H48" s="24">
-        <v>0.47805999999999998</v>
+        <v>27.59</v>
       </c>
       <c r="I48" s="24">
-        <v>0.13603999999999999</v>
-      </c>
-      <c r="J48" s="42">
-        <v>5.04</v>
-      </c>
-      <c r="K48" s="42">
-        <v>0.86</v>
-      </c>
-      <c r="L48" s="42">
-        <v>2.96</v>
+        <v>0.38627</v>
+      </c>
+      <c r="J48" s="12">
+        <v>42.84</v>
+      </c>
+      <c r="K48" s="12">
+        <v>17.04</v>
+      </c>
+      <c r="L48" s="12">
+        <v>34.15</v>
       </c>
       <c r="M48" s="42">
-        <v>1.22</v>
-      </c>
-      <c r="N48" s="42">
-        <v>0.19</v>
+        <v>19.96</v>
+      </c>
+      <c r="N48" s="12">
+        <v>6.93</v>
       </c>
       <c r="O48" s="21">
-        <v>2.3599999999999999E-2</v>
+        <v>0.17230000000000001</v>
       </c>
       <c r="P48" s="21">
-        <v>-1.3100000000000001E-2</v>
+        <v>0.22109999999999999</v>
       </c>
       <c r="Q48" s="21">
-        <v>5.2699999999999997E-2</v>
+        <v>0.2641</v>
       </c>
       <c r="R48" s="21">
-        <v>0.16619999999999999</v>
+        <v>0.39879999999999999</v>
       </c>
       <c r="S48" s="21">
-        <v>1.8692</v>
-      </c>
-      <c r="T48" s="45">
-        <v>1.51</v>
-      </c>
-      <c r="U48" s="74"/>
+        <v>0.379</v>
+      </c>
+      <c r="T48" s="35">
+        <v>2.56</v>
+      </c>
+      <c r="U48" s="44"/>
       <c r="V48" s="13" t="s">
-        <v>335</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="1:22">
       <c r="A49" s="18"/>
       <c r="B49" s="11" t="s">
-        <v>425</v>
+        <v>334</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="34" t="s">
-        <v>426</v>
+        <v>333</v>
       </c>
       <c r="H49" s="24">
-        <v>2.86</v>
+        <v>0.47805999999999998</v>
       </c>
       <c r="I49" s="24">
-        <v>0.77800000000000002</v>
-      </c>
-      <c r="J49" s="42"/>
-      <c r="K49" s="42"/>
+        <v>0.13603999999999999</v>
+      </c>
+      <c r="J49" s="42">
+        <v>5.04</v>
+      </c>
+      <c r="K49" s="42">
+        <v>0.86</v>
+      </c>
       <c r="L49" s="42">
-        <v>12.83</v>
+        <v>2.96</v>
       </c>
       <c r="M49" s="42">
-        <v>-15.19</v>
+        <v>1.22</v>
       </c>
       <c r="N49" s="42">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="O49" s="21">
-        <v>2.4299999999999999E-2</v>
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="P49" s="21">
-        <v>-0.31569999999999998</v>
+        <v>-1.3100000000000001E-2</v>
       </c>
       <c r="Q49" s="21">
-        <v>0.12130000000000001</v>
-      </c>
-      <c r="R49" s="46">
-        <v>0.31990000000000002</v>
+        <v>5.2699999999999997E-2</v>
+      </c>
+      <c r="R49" s="21">
+        <v>0.16619999999999999</v>
       </c>
       <c r="S49" s="21">
-        <v>-6.07</v>
+        <v>1.8692</v>
       </c>
       <c r="T49" s="45">
-        <v>1.26</v>
+        <v>1.51</v>
       </c>
       <c r="U49" s="74"/>
       <c r="V49" s="13" t="s">
@@ -38370,722 +38395,852 @@
     <row r="50" spans="1:22">
       <c r="A50" s="18"/>
       <c r="B50" s="11" t="s">
-        <v>554</v>
+        <v>425</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="12"/>
       <c r="G50" s="34" t="s">
-        <v>553</v>
+        <v>426</v>
       </c>
       <c r="H50" s="24">
-        <v>4.3099999999999996</v>
+        <v>2.86</v>
       </c>
       <c r="I50" s="24">
-        <v>-0.16614999999999999</v>
-      </c>
-      <c r="K50" s="42">
-        <v>3.39</v>
-      </c>
-      <c r="L50" s="42"/>
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="J50" s="42"/>
+      <c r="K50" s="42"/>
+      <c r="L50" s="42">
+        <v>12.83</v>
+      </c>
       <c r="M50" s="42">
-        <v>-16.11</v>
+        <v>-15.19</v>
       </c>
       <c r="N50" s="42">
-        <v>3.85</v>
+        <v>0.22</v>
       </c>
       <c r="O50" s="21">
-        <v>0.33350000000000002</v>
+        <v>2.4299999999999999E-2</v>
       </c>
       <c r="P50" s="21">
-        <v>0.29530000000000001</v>
+        <v>-0.31569999999999998</v>
       </c>
       <c r="Q50" s="21">
-        <v>-0.27400000000000002</v>
+        <v>0.12130000000000001</v>
       </c>
       <c r="R50" s="46">
-        <v>-0.3322</v>
+        <v>0.31990000000000002</v>
       </c>
       <c r="S50" s="21">
-        <v>0.1022</v>
+        <v>-6.07</v>
       </c>
       <c r="T50" s="45">
-        <v>2.35</v>
-      </c>
-      <c r="U50" s="74">
-        <v>225300</v>
-      </c>
+        <v>1.26</v>
+      </c>
+      <c r="U50" s="74"/>
       <c r="V50" s="13" t="s">
-        <v>555</v>
+        <v>335</v>
       </c>
     </row>
     <row r="51" spans="1:22">
       <c r="A51" s="18"/>
-      <c r="B51" s="11"/>
+      <c r="B51" s="11" t="s">
+        <v>554</v>
+      </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="42"/>
+      <c r="G51" s="34" t="s">
+        <v>553</v>
+      </c>
+      <c r="H51" s="24">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="I51" s="24">
+        <v>-0.16614999999999999</v>
+      </c>
+      <c r="K51" s="42">
+        <v>3.39</v>
+      </c>
       <c r="L51" s="42"/>
-      <c r="M51" s="42"/>
-      <c r="N51" s="42"/>
-      <c r="O51" s="21"/>
-      <c r="P51" s="21"/>
-      <c r="Q51" s="21"/>
-      <c r="R51" s="46"/>
-      <c r="S51" s="21"/>
-      <c r="T51" s="45"/>
-      <c r="U51" s="74"/>
-      <c r="V51" s="13"/>
+      <c r="M51" s="42">
+        <v>-16.11</v>
+      </c>
+      <c r="N51" s="42">
+        <v>3.85</v>
+      </c>
+      <c r="O51" s="21">
+        <v>0.33350000000000002</v>
+      </c>
+      <c r="P51" s="21">
+        <v>0.29530000000000001</v>
+      </c>
+      <c r="Q51" s="21">
+        <v>-0.27400000000000002</v>
+      </c>
+      <c r="R51" s="46">
+        <v>-0.3322</v>
+      </c>
+      <c r="S51" s="21">
+        <v>0.1022</v>
+      </c>
+      <c r="T51" s="45">
+        <v>2.35</v>
+      </c>
+      <c r="U51" s="74">
+        <v>225300</v>
+      </c>
+      <c r="V51" s="13" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="52" spans="1:22">
-      <c r="A52" s="19"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15"/>
-      <c r="F52" s="15"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="39"/>
-      <c r="I52" s="15"/>
-      <c r="J52" s="15"/>
-      <c r="K52" s="15"/>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="22"/>
-      <c r="Q52" s="22"/>
-      <c r="R52" s="22"/>
-      <c r="S52" s="22"/>
-      <c r="T52" s="37"/>
-      <c r="U52" s="53"/>
-      <c r="V52" s="16"/>
+      <c r="A52" s="18"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="42"/>
+      <c r="K52" s="42"/>
+      <c r="L52" s="42"/>
+      <c r="M52" s="42"/>
+      <c r="N52" s="42"/>
+      <c r="O52" s="21"/>
+      <c r="P52" s="21"/>
+      <c r="Q52" s="21"/>
+      <c r="R52" s="46"/>
+      <c r="S52" s="21"/>
+      <c r="T52" s="45"/>
+      <c r="U52" s="74"/>
+      <c r="V52" s="13"/>
     </row>
     <row r="53" spans="1:22">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="19"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="22"/>
+      <c r="P53" s="22"/>
+      <c r="Q53" s="22"/>
+      <c r="R53" s="22"/>
+      <c r="S53" s="22"/>
+      <c r="T53" s="37"/>
+      <c r="U53" s="53"/>
+      <c r="V53" s="16"/>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B54" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="28" t="s">
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="28" t="s">
         <v>302</v>
       </c>
-      <c r="H53" s="38">
+      <c r="H54" s="38">
         <v>83.02</v>
       </c>
-      <c r="I53" s="38">
+      <c r="I54" s="38">
         <v>5.37</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J54" s="9">
         <v>18.48</v>
       </c>
-      <c r="K53" s="9">
+      <c r="K54" s="9">
         <v>8.19</v>
       </c>
-      <c r="L53" s="9">
+      <c r="L54" s="9">
         <v>13.48</v>
       </c>
-      <c r="M53" s="9"/>
-      <c r="N53" s="9">
+      <c r="M54" s="9"/>
+      <c r="N54" s="9">
         <v>2.58</v>
       </c>
-      <c r="O53" s="20">
+      <c r="O54" s="20">
         <v>2E-3</v>
       </c>
-      <c r="P53" s="20">
+      <c r="P54" s="20">
         <v>-6.4000000000000003E-3</v>
       </c>
-      <c r="Q53" s="20">
+      <c r="Q54" s="20">
         <v>0.26950000000000002</v>
       </c>
-      <c r="R53" s="20">
+      <c r="R54" s="20">
         <v>0.45079999999999998</v>
       </c>
-      <c r="S53" s="20">
+      <c r="S54" s="20">
         <v>2.1166</v>
       </c>
-      <c r="T53" s="29">
+      <c r="T54" s="29">
         <v>1.89</v>
       </c>
-      <c r="U53" s="43">
+      <c r="U54" s="43">
         <v>336390</v>
       </c>
-      <c r="V53" s="10" t="s">
+      <c r="V54" s="10" t="s">
         <v>304</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22">
-      <c r="A54" s="18"/>
-      <c r="B54" s="11" t="s">
-        <v>325</v>
-      </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="34" t="s">
-        <v>305</v>
-      </c>
-      <c r="H54" s="24">
-        <v>295.58999999999997</v>
-      </c>
-      <c r="I54" s="24">
-        <v>13.52</v>
-      </c>
-      <c r="J54" s="12">
-        <v>67.459999999999994</v>
-      </c>
-      <c r="K54" s="12">
-        <v>6.4</v>
-      </c>
-      <c r="L54" s="12">
-        <v>37.08</v>
-      </c>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12">
-        <v>4.22</v>
-      </c>
-      <c r="O54" s="21">
-        <v>-4.0099999999999997E-2</v>
-      </c>
-      <c r="P54" s="21">
-        <v>-0.14499999999999999</v>
-      </c>
-      <c r="Q54" s="21">
-        <v>0.27189999999999998</v>
-      </c>
-      <c r="R54" s="21">
-        <v>0.1018</v>
-      </c>
-      <c r="S54" s="21">
-        <v>0.80710000000000004</v>
-      </c>
-      <c r="T54" s="35">
-        <v>0.73</v>
-      </c>
-      <c r="U54" s="44">
-        <v>725220</v>
-      </c>
-      <c r="V54" s="13" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:22">
       <c r="A55" s="18"/>
       <c r="B55" s="11" t="s">
-        <v>521</v>
-      </c>
-      <c r="C55" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F55" s="12" t="s">
-        <v>9</v>
-      </c>
+        <v>325</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
       <c r="G55" s="34" t="s">
-        <v>522</v>
+        <v>305</v>
       </c>
       <c r="H55" s="24">
-        <v>46.61</v>
+        <v>295.58999999999997</v>
       </c>
       <c r="I55" s="24">
-        <v>1.88</v>
+        <v>13.52</v>
       </c>
       <c r="J55" s="12">
-        <v>19.97</v>
-      </c>
-      <c r="K55" s="12"/>
+        <v>67.459999999999994</v>
+      </c>
+      <c r="K55" s="12">
+        <v>6.4</v>
+      </c>
       <c r="L55" s="12">
-        <v>14.37</v>
-      </c>
-      <c r="M55" s="42">
-        <v>13.35</v>
-      </c>
-      <c r="N55" s="42">
-        <v>2.4900000000000002</v>
+        <v>37.08</v>
+      </c>
+      <c r="M55" s="12"/>
+      <c r="N55" s="12">
+        <v>4.22</v>
       </c>
       <c r="O55" s="21">
-        <v>-1.3299999999999999E-2</v>
+        <v>-4.0099999999999997E-2</v>
       </c>
       <c r="P55" s="21">
-        <v>6.2600000000000003E-2</v>
+        <v>-0.14499999999999999</v>
       </c>
       <c r="Q55" s="21">
-        <v>0.23319999999999999</v>
+        <v>0.27189999999999998</v>
       </c>
       <c r="R55" s="21">
-        <v>-18.2119</v>
+        <v>0.1018</v>
       </c>
       <c r="S55" s="21">
-        <v>-50.586799999999997</v>
+        <v>0.80710000000000004</v>
       </c>
       <c r="T55" s="35">
-        <v>0.79</v>
+        <v>0.73</v>
       </c>
       <c r="U55" s="44">
-        <v>470650</v>
+        <v>725220</v>
       </c>
       <c r="V55" s="13" t="s">
-        <v>523</v>
+        <v>306</v>
       </c>
     </row>
     <row r="56" spans="1:22">
       <c r="A56" s="18"/>
       <c r="B56" s="11" t="s">
-        <v>524</v>
-      </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+        <v>521</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="G56" s="34" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="H56" s="24">
-        <v>2.63</v>
+        <v>46.61</v>
       </c>
       <c r="I56" s="24">
-        <v>9.2100000000000001E-2</v>
-      </c>
-      <c r="J56" s="42">
-        <v>118.56</v>
-      </c>
-      <c r="K56" s="12">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="L56" s="42">
-        <v>17.690000000000001</v>
+        <v>1.88</v>
+      </c>
+      <c r="J56" s="12">
+        <v>19.97</v>
+      </c>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12">
+        <v>14.37</v>
       </c>
       <c r="M56" s="42">
-        <v>8.9499999999999993</v>
+        <v>13.35</v>
       </c>
       <c r="N56" s="42">
-        <v>0.99</v>
+        <v>2.4900000000000002</v>
       </c>
       <c r="O56" s="21">
-        <v>6.2700000000000006E-2</v>
+        <v>-1.3299999999999999E-2</v>
       </c>
       <c r="P56" s="21">
-        <v>-4.2599999999999999E-2</v>
+        <v>6.2600000000000003E-2</v>
       </c>
       <c r="Q56" s="21">
-        <v>0.19689999999999999</v>
+        <v>0.23319999999999999</v>
       </c>
       <c r="R56" s="21">
-        <v>4.0399999999999998E-2</v>
+        <v>-18.2119</v>
       </c>
       <c r="S56" s="21">
-        <v>6.0693999999999999</v>
+        <v>-50.586799999999997</v>
       </c>
       <c r="T56" s="35">
-        <v>1.93</v>
+        <v>0.79</v>
       </c>
       <c r="U56" s="44">
-        <v>354590</v>
+        <v>470650</v>
       </c>
       <c r="V56" s="13" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="57" spans="1:22">
       <c r="A57" s="18"/>
       <c r="B57" s="11" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="34" t="s">
+        <v>525</v>
+      </c>
+      <c r="H57" s="24">
+        <v>2.63</v>
+      </c>
+      <c r="I57" s="24">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="J57" s="42">
+        <v>118.56</v>
+      </c>
+      <c r="K57" s="12">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="L57" s="42">
+        <v>17.690000000000001</v>
+      </c>
+      <c r="M57" s="42">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="N57" s="42">
+        <v>0.99</v>
+      </c>
+      <c r="O57" s="21">
+        <v>6.2700000000000006E-2</v>
+      </c>
+      <c r="P57" s="21">
+        <v>-4.2599999999999999E-2</v>
+      </c>
+      <c r="Q57" s="21">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="R57" s="21">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="S57" s="21">
+        <v>6.0693999999999999</v>
+      </c>
+      <c r="T57" s="35">
+        <v>1.93</v>
+      </c>
+      <c r="U57" s="44">
+        <v>354590</v>
+      </c>
+      <c r="V57" s="13" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22">
+      <c r="A58" s="18"/>
+      <c r="B58" s="11" t="s">
+        <v>534</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="34" t="s">
         <v>533</v>
       </c>
-      <c r="H57" s="24">
+      <c r="H58" s="24">
         <v>128.51</v>
       </c>
-      <c r="I57" s="24">
+      <c r="I58" s="24">
         <v>7.62</v>
       </c>
-      <c r="J57" s="12"/>
-      <c r="K57" s="42">
+      <c r="J58" s="12"/>
+      <c r="K58" s="42">
         <v>8.7799999999999994</v>
       </c>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12">
+      <c r="L58" s="12"/>
+      <c r="M58" s="12">
         <v>15.99</v>
       </c>
-      <c r="N57" s="42">
+      <c r="N58" s="42">
         <v>2.2000000000000002</v>
       </c>
-      <c r="O57" s="21">
+      <c r="O58" s="21">
         <v>-1E-3</v>
       </c>
-      <c r="P57" s="21">
+      <c r="P58" s="21">
         <v>2.29E-2</v>
       </c>
-      <c r="Q57" s="21"/>
-      <c r="R57" s="21"/>
-      <c r="S57" s="21">
+      <c r="Q58" s="21"/>
+      <c r="R58" s="21"/>
+      <c r="S58" s="21">
         <v>2.1076000000000001</v>
       </c>
-      <c r="T57" s="35">
+      <c r="T58" s="35">
         <v>0.8</v>
       </c>
-      <c r="U57" s="44">
+      <c r="U58" s="44">
         <v>389220</v>
       </c>
-      <c r="V57" s="13" t="s">
+      <c r="V58" s="13" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="58" spans="1:22">
-      <c r="A58" s="19"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="15"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="22"/>
-      <c r="Q58" s="22"/>
-      <c r="R58" s="22"/>
-      <c r="S58" s="22"/>
-      <c r="T58" s="37"/>
-      <c r="U58" s="15"/>
-      <c r="V58" s="16"/>
-    </row>
     <row r="59" spans="1:22">
-      <c r="A59" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="B59" t="s">
-        <v>316</v>
-      </c>
-      <c r="G59" t="s">
-        <v>315</v>
-      </c>
-      <c r="H59">
-        <v>5.35</v>
-      </c>
-      <c r="I59">
-        <v>2.7E-2</v>
-      </c>
-      <c r="J59">
-        <v>7.24</v>
-      </c>
-      <c r="K59">
-        <v>1.46</v>
-      </c>
-      <c r="L59">
-        <v>4.99</v>
-      </c>
-      <c r="M59">
-        <v>3.32</v>
-      </c>
-      <c r="N59">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="O59">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="P59">
-        <v>9.4200000000000006E-2</v>
-      </c>
-      <c r="Q59">
-        <v>0.10920000000000001</v>
-      </c>
-      <c r="R59">
-        <v>0.20449999999999999</v>
-      </c>
-      <c r="S59">
-        <v>0.51690000000000003</v>
-      </c>
-      <c r="T59">
-        <v>1.33</v>
-      </c>
-      <c r="V59" s="79" t="s">
-        <v>314</v>
+      <c r="A59" s="18"/>
+      <c r="B59" s="11" t="s">
+        <v>653</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="34" t="s">
+        <v>652</v>
+      </c>
+      <c r="H59" s="24">
+        <v>69.87</v>
+      </c>
+      <c r="I59" s="24">
+        <v>8.42</v>
+      </c>
+      <c r="J59" s="12"/>
+      <c r="K59" s="42">
+        <v>7.42</v>
+      </c>
+      <c r="L59" s="12"/>
+      <c r="M59" s="42">
+        <v>10.8</v>
+      </c>
+      <c r="N59" s="42">
+        <v>3.43</v>
+      </c>
+      <c r="O59" s="21">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="P59" s="21">
+        <v>-0.2737</v>
+      </c>
+      <c r="Q59" s="21">
+        <v>0.54820000000000002</v>
+      </c>
+      <c r="R59" s="21">
+        <v>-9.1200000000000003E-2</v>
+      </c>
+      <c r="S59" s="21">
+        <v>4.5805999999999996</v>
+      </c>
+      <c r="T59" s="35">
+        <v>0.62</v>
+      </c>
+      <c r="U59" s="44">
+        <v>2801780</v>
+      </c>
+      <c r="V59" s="13" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="60" spans="1:22">
       <c r="A60" s="18"/>
-      <c r="B60" s="56" t="s">
-        <v>318</v>
-      </c>
-      <c r="C60" s="56"/>
-      <c r="D60" s="56"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="54" t="s">
-        <v>317</v>
-      </c>
-      <c r="H60" s="55">
-        <v>7.01</v>
-      </c>
-      <c r="I60" s="55">
-        <v>1.07</v>
-      </c>
-      <c r="J60" s="56">
-        <v>3.52</v>
-      </c>
-      <c r="K60" s="56">
-        <v>1.07</v>
-      </c>
-      <c r="L60" s="56">
-        <v>2.16</v>
-      </c>
-      <c r="M60" s="56">
-        <v>0.75</v>
-      </c>
-      <c r="N60" s="56">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="O60" s="57">
-        <v>5.0500000000000003E-2</v>
-      </c>
-      <c r="P60" s="57">
-        <v>0.38150000000000001</v>
-      </c>
-      <c r="Q60" s="57">
-        <v>0.20930000000000001</v>
-      </c>
-      <c r="R60" s="57">
-        <v>0.30209999999999998</v>
-      </c>
-      <c r="S60" s="57">
-        <v>2.0200999999999998</v>
-      </c>
-      <c r="T60" s="56">
-        <v>0.92</v>
-      </c>
-      <c r="U60" s="73">
-        <v>147850</v>
-      </c>
-      <c r="V60" s="68" t="s">
+      <c r="B60" s="11"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="24"/>
+      <c r="I60" s="24"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="42"/>
+      <c r="L60" s="12"/>
+      <c r="M60" s="42"/>
+      <c r="N60" s="42"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="21"/>
+      <c r="Q60" s="21"/>
+      <c r="R60" s="21"/>
+      <c r="S60" s="21"/>
+      <c r="T60" s="35"/>
+      <c r="U60" s="44"/>
+      <c r="V60" s="13"/>
+    </row>
+    <row r="61" spans="1:22">
+      <c r="A61" s="19"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="22"/>
+      <c r="S61" s="22"/>
+      <c r="T61" s="37"/>
+      <c r="U61" s="15"/>
+      <c r="V61" s="16"/>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="A62" s="17" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="61" spans="1:22">
-      <c r="A61" s="18"/>
-      <c r="B61" s="60" t="s">
-        <v>320</v>
-      </c>
-      <c r="C61" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D61" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F61" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G61" s="34" t="s">
-        <v>319</v>
-      </c>
-      <c r="H61" s="24">
-        <v>8.23</v>
-      </c>
-      <c r="I61" s="24">
-        <v>-0.16222</v>
-      </c>
-      <c r="J61" s="42">
-        <v>66.62</v>
-      </c>
-      <c r="K61" s="42">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="L61" s="42">
-        <v>11.01</v>
-      </c>
-      <c r="M61" s="42">
-        <v>20.14</v>
-      </c>
-      <c r="N61" s="42">
-        <v>1.25</v>
-      </c>
-      <c r="O61" s="21">
-        <v>0.04</v>
-      </c>
-      <c r="P61" s="21">
-        <v>-6.4799999999999996E-2</v>
-      </c>
-      <c r="Q61" s="21">
-        <v>0.23269999999999999</v>
-      </c>
-      <c r="R61" s="21">
-        <v>6.3100000000000003E-2</v>
-      </c>
-      <c r="S61" s="21">
-        <v>6.0811999999999999</v>
-      </c>
-      <c r="T61" s="12">
-        <v>1.18</v>
-      </c>
-      <c r="U61" s="12"/>
-      <c r="V61" s="13" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="62" spans="1:22">
-      <c r="A62" s="18"/>
-      <c r="B62" s="60" t="s">
-        <v>321</v>
-      </c>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="34" t="s">
-        <v>322</v>
-      </c>
-      <c r="H62" s="24">
-        <v>19.91</v>
-      </c>
-      <c r="I62" s="24">
-        <v>1.3</v>
-      </c>
-      <c r="J62" s="42">
-        <v>23.48</v>
-      </c>
-      <c r="K62" s="12"/>
-      <c r="L62" s="42">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="M62" s="42">
-        <v>18.78</v>
-      </c>
-      <c r="N62" s="42">
-        <v>2.16</v>
-      </c>
-      <c r="O62" s="21">
-        <v>-2.0799999999999999E-2</v>
-      </c>
-      <c r="P62" s="21">
-        <v>-1.1599999999999999E-2</v>
-      </c>
-      <c r="Q62" s="21">
-        <v>0.20369999999999999</v>
-      </c>
-      <c r="R62" s="21">
-        <v>-5.6839000000000004</v>
-      </c>
-      <c r="S62" s="21">
-        <v>-19.010400000000001</v>
-      </c>
-      <c r="T62" s="35">
-        <v>0.74</v>
-      </c>
-      <c r="U62" s="35"/>
-      <c r="V62" s="13" t="s">
+      <c r="B62" t="s">
+        <v>316</v>
+      </c>
+      <c r="G62" t="s">
+        <v>315</v>
+      </c>
+      <c r="H62">
+        <v>5.35</v>
+      </c>
+      <c r="I62">
+        <v>2.7E-2</v>
+      </c>
+      <c r="J62">
+        <v>7.24</v>
+      </c>
+      <c r="K62">
+        <v>1.46</v>
+      </c>
+      <c r="L62">
+        <v>4.99</v>
+      </c>
+      <c r="M62">
+        <v>3.32</v>
+      </c>
+      <c r="N62">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="O62">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="P62">
+        <v>9.4200000000000006E-2</v>
+      </c>
+      <c r="Q62">
+        <v>0.10920000000000001</v>
+      </c>
+      <c r="R62">
+        <v>0.20449999999999999</v>
+      </c>
+      <c r="S62">
+        <v>0.51690000000000003</v>
+      </c>
+      <c r="T62">
+        <v>1.33</v>
+      </c>
+      <c r="V62" s="79" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:22">
       <c r="A63" s="18"/>
-      <c r="B63" s="60" t="s">
+      <c r="B63" s="109" t="s">
+        <v>318</v>
+      </c>
+      <c r="C63" s="109"/>
+      <c r="D63" s="109"/>
+      <c r="E63" s="109"/>
+      <c r="F63" s="109"/>
+      <c r="G63" s="110" t="s">
+        <v>317</v>
+      </c>
+      <c r="H63" s="111">
+        <v>7.01</v>
+      </c>
+      <c r="I63" s="111">
+        <v>1.07</v>
+      </c>
+      <c r="J63" s="109">
+        <v>3.52</v>
+      </c>
+      <c r="K63" s="109">
+        <v>1.07</v>
+      </c>
+      <c r="L63" s="109">
+        <v>2.16</v>
+      </c>
+      <c r="M63" s="109">
+        <v>0.75</v>
+      </c>
+      <c r="N63" s="109">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="O63" s="112">
+        <v>5.0500000000000003E-2</v>
+      </c>
+      <c r="P63" s="112">
+        <v>0.38150000000000001</v>
+      </c>
+      <c r="Q63" s="112">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="R63" s="112">
+        <v>0.30209999999999998</v>
+      </c>
+      <c r="S63" s="112">
+        <v>2.0200999999999998</v>
+      </c>
+      <c r="T63" s="109">
+        <v>0.92</v>
+      </c>
+      <c r="U63" s="114">
+        <v>147850</v>
+      </c>
+      <c r="V63" s="113" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
+      <c r="A64" s="18"/>
+      <c r="B64" s="60" t="s">
+        <v>320</v>
+      </c>
+      <c r="C64" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="H64" s="24">
+        <v>8.23</v>
+      </c>
+      <c r="I64" s="24">
+        <v>-0.16222</v>
+      </c>
+      <c r="J64" s="42">
+        <v>66.62</v>
+      </c>
+      <c r="K64" s="42">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="L64" s="42">
+        <v>11.01</v>
+      </c>
+      <c r="M64" s="42">
+        <v>20.14</v>
+      </c>
+      <c r="N64" s="42">
+        <v>1.25</v>
+      </c>
+      <c r="O64" s="21">
+        <v>0.04</v>
+      </c>
+      <c r="P64" s="21">
+        <v>-6.4799999999999996E-2</v>
+      </c>
+      <c r="Q64" s="21">
+        <v>0.23269999999999999</v>
+      </c>
+      <c r="R64" s="21">
+        <v>6.3100000000000003E-2</v>
+      </c>
+      <c r="S64" s="21">
+        <v>6.0811999999999999</v>
+      </c>
+      <c r="T64" s="12">
+        <v>1.18</v>
+      </c>
+      <c r="U64" s="12"/>
+      <c r="V64" s="13" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65" s="18"/>
+      <c r="B65" s="60" t="s">
+        <v>321</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="H65" s="24">
+        <v>19.91</v>
+      </c>
+      <c r="I65" s="24">
+        <v>1.3</v>
+      </c>
+      <c r="J65" s="42">
+        <v>23.48</v>
+      </c>
+      <c r="K65" s="12"/>
+      <c r="L65" s="42">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="M65" s="42">
+        <v>18.78</v>
+      </c>
+      <c r="N65" s="42">
+        <v>2.16</v>
+      </c>
+      <c r="O65" s="21">
+        <v>-2.0799999999999999E-2</v>
+      </c>
+      <c r="P65" s="21">
+        <v>-1.1599999999999999E-2</v>
+      </c>
+      <c r="Q65" s="21">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="R65" s="21">
+        <v>-5.6839000000000004</v>
+      </c>
+      <c r="S65" s="21">
+        <v>-19.010400000000001</v>
+      </c>
+      <c r="T65" s="35">
+        <v>0.74</v>
+      </c>
+      <c r="U65" s="35"/>
+      <c r="V65" s="13" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" s="18"/>
+      <c r="B66" s="60" t="s">
         <v>323</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="34" t="s">
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="H63" s="24">
+      <c r="H66" s="24">
         <v>26.15</v>
       </c>
-      <c r="I63" s="24">
+      <c r="I66" s="24">
         <v>1.03</v>
       </c>
-      <c r="J63" s="42">
+      <c r="J66" s="42">
         <v>21.3</v>
       </c>
-      <c r="K63" s="42">
+      <c r="K66" s="42">
         <v>24.22</v>
       </c>
-      <c r="L63" s="42">
+      <c r="L66" s="42">
         <v>16.38</v>
       </c>
-      <c r="M63" s="42">
+      <c r="M66" s="42">
         <v>17.53</v>
       </c>
-      <c r="N63" s="42">
+      <c r="N66" s="42">
         <v>1.27</v>
       </c>
-      <c r="O63" s="21">
+      <c r="O66" s="21">
         <v>8.7400000000000005E-2</v>
       </c>
-      <c r="P63" s="21">
+      <c r="P66" s="21">
         <v>0.1183</v>
       </c>
-      <c r="Q63" s="21">
+      <c r="Q66" s="21">
         <v>0.1144</v>
       </c>
-      <c r="R63" s="21">
+      <c r="R66" s="21">
         <v>1.1615</v>
       </c>
-      <c r="S63" s="21">
+      <c r="S66" s="21">
         <v>17.0014</v>
       </c>
-      <c r="T63" s="35">
+      <c r="T66" s="35">
         <v>0.49</v>
       </c>
-      <c r="U63" s="35"/>
-      <c r="V63" s="13" t="s">
+      <c r="U66" s="35"/>
+      <c r="V66" s="13" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="64" spans="1:22">
-      <c r="A64" s="19"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="36"/>
-      <c r="H64" s="39"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="22"/>
-      <c r="Q64" s="22"/>
-      <c r="R64" s="22"/>
-      <c r="S64" s="22"/>
-      <c r="T64" s="37"/>
-      <c r="U64" s="37"/>
-      <c r="V64" s="16"/>
+    <row r="67" spans="1:22">
+      <c r="A67" s="19"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="39"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="22"/>
+      <c r="P67" s="22"/>
+      <c r="Q67" s="22"/>
+      <c r="R67" s="22"/>
+      <c r="S67" s="22"/>
+      <c r="T67" s="37"/>
+      <c r="U67" s="37"/>
+      <c r="V67" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>